<commit_message>
tp sl for ce being changed
</commit_message>
<xml_diff>
--- a/storage/Ibkr.xlsx
+++ b/storage/Ibkr.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K113"/>
+  <dimension ref="A1:K132"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4869,6 +4869,747 @@
         <v>0</v>
       </c>
     </row>
+    <row r="114">
+      <c r="A114" t="n">
+        <v>37000</v>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>MARKET</t>
+        </is>
+      </c>
+      <c r="C114" t="n">
+        <v>38800</v>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E114" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F114" t="n">
+        <v>38810</v>
+      </c>
+      <c r="G114" t="n">
+        <v>38700</v>
+      </c>
+      <c r="H114" t="n">
+        <v>10</v>
+      </c>
+      <c r="I114" t="n">
+        <v>2</v>
+      </c>
+      <c r="J114" t="n">
+        <v>5</v>
+      </c>
+      <c r="K114" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="n">
+        <v>37000</v>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>MARKET</t>
+        </is>
+      </c>
+      <c r="C115" t="n">
+        <v>38800</v>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E115" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F115" t="n">
+        <v>38810</v>
+      </c>
+      <c r="G115" t="n">
+        <v>38700</v>
+      </c>
+      <c r="H115" t="n">
+        <v>10</v>
+      </c>
+      <c r="I115" t="n">
+        <v>2</v>
+      </c>
+      <c r="J115" t="n">
+        <v>5</v>
+      </c>
+      <c r="K115" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="n">
+        <v>37000</v>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>MARKET</t>
+        </is>
+      </c>
+      <c r="C116" t="n">
+        <v>38800</v>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E116" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F116" t="n">
+        <v>38810</v>
+      </c>
+      <c r="G116" t="n">
+        <v>38700</v>
+      </c>
+      <c r="H116" t="n">
+        <v>10</v>
+      </c>
+      <c r="I116" t="n">
+        <v>2</v>
+      </c>
+      <c r="J116" t="n">
+        <v>5</v>
+      </c>
+      <c r="K116" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="n">
+        <v>37000</v>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>MARKET</t>
+        </is>
+      </c>
+      <c r="C117" t="n">
+        <v>39000</v>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E117" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F117" t="n">
+        <v>39100</v>
+      </c>
+      <c r="G117" t="n">
+        <v>38700</v>
+      </c>
+      <c r="H117" t="n">
+        <v>10</v>
+      </c>
+      <c r="I117" t="n">
+        <v>2</v>
+      </c>
+      <c r="J117" t="n">
+        <v>5</v>
+      </c>
+      <c r="K117" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="n">
+        <v>37000</v>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>MARKET</t>
+        </is>
+      </c>
+      <c r="C118" t="n">
+        <v>39000</v>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E118" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F118" t="n">
+        <v>39100</v>
+      </c>
+      <c r="G118" t="n">
+        <v>38700</v>
+      </c>
+      <c r="H118" t="n">
+        <v>10</v>
+      </c>
+      <c r="I118" t="n">
+        <v>2</v>
+      </c>
+      <c r="J118" t="n">
+        <v>5</v>
+      </c>
+      <c r="K118" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="n">
+        <v>37000</v>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>MARKET</t>
+        </is>
+      </c>
+      <c r="C119" t="n">
+        <v>39000</v>
+      </c>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E119" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F119" t="n">
+        <v>39100</v>
+      </c>
+      <c r="G119" t="n">
+        <v>38700</v>
+      </c>
+      <c r="H119" t="n">
+        <v>10</v>
+      </c>
+      <c r="I119" t="n">
+        <v>2</v>
+      </c>
+      <c r="J119" t="n">
+        <v>5</v>
+      </c>
+      <c r="K119" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="n">
+        <v>37000</v>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>MARKET</t>
+        </is>
+      </c>
+      <c r="C120" t="n">
+        <v>39000</v>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E120" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F120" t="n">
+        <v>39100</v>
+      </c>
+      <c r="G120" t="n">
+        <v>38700</v>
+      </c>
+      <c r="H120" t="n">
+        <v>10</v>
+      </c>
+      <c r="I120" t="n">
+        <v>2</v>
+      </c>
+      <c r="J120" t="n">
+        <v>5</v>
+      </c>
+      <c r="K120" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="n">
+        <v>37000</v>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>MARKET</t>
+        </is>
+      </c>
+      <c r="C121" t="n">
+        <v>39000</v>
+      </c>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E121" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F121" t="n">
+        <v>39100</v>
+      </c>
+      <c r="G121" t="n">
+        <v>38700</v>
+      </c>
+      <c r="H121" t="n">
+        <v>10</v>
+      </c>
+      <c r="I121" t="n">
+        <v>2</v>
+      </c>
+      <c r="J121" t="n">
+        <v>5</v>
+      </c>
+      <c r="K121" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="n">
+        <v>37000</v>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>MARKET</t>
+        </is>
+      </c>
+      <c r="C122" t="n">
+        <v>39000</v>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E122" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F122" t="n">
+        <v>39100</v>
+      </c>
+      <c r="G122" t="n">
+        <v>38700</v>
+      </c>
+      <c r="H122" t="n">
+        <v>10</v>
+      </c>
+      <c r="I122" t="n">
+        <v>2</v>
+      </c>
+      <c r="J122" t="n">
+        <v>5</v>
+      </c>
+      <c r="K122" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="n">
+        <v>37000</v>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>MARKET</t>
+        </is>
+      </c>
+      <c r="C123" t="n">
+        <v>39000</v>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E123" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F123" t="n">
+        <v>39100</v>
+      </c>
+      <c r="G123" t="n">
+        <v>38700</v>
+      </c>
+      <c r="H123" t="n">
+        <v>10</v>
+      </c>
+      <c r="I123" t="n">
+        <v>2</v>
+      </c>
+      <c r="J123" t="n">
+        <v>5</v>
+      </c>
+      <c r="K123" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="n">
+        <v>37000</v>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>MARKET</t>
+        </is>
+      </c>
+      <c r="C124" t="n">
+        <v>39000</v>
+      </c>
+      <c r="D124" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E124" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F124" t="n">
+        <v>39100</v>
+      </c>
+      <c r="G124" t="n">
+        <v>38700</v>
+      </c>
+      <c r="H124" t="n">
+        <v>10</v>
+      </c>
+      <c r="I124" t="n">
+        <v>2</v>
+      </c>
+      <c r="J124" t="n">
+        <v>5</v>
+      </c>
+      <c r="K124" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="n">
+        <v>37000</v>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>MARKET</t>
+        </is>
+      </c>
+      <c r="C125" t="n">
+        <v>39000</v>
+      </c>
+      <c r="D125" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E125" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F125" t="n">
+        <v>39100</v>
+      </c>
+      <c r="G125" t="n">
+        <v>38700</v>
+      </c>
+      <c r="H125" t="n">
+        <v>10</v>
+      </c>
+      <c r="I125" t="n">
+        <v>2</v>
+      </c>
+      <c r="J125" t="n">
+        <v>5</v>
+      </c>
+      <c r="K125" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="n">
+        <v>37000</v>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>MARKET</t>
+        </is>
+      </c>
+      <c r="C126" t="n">
+        <v>39000</v>
+      </c>
+      <c r="D126" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E126" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F126" t="n">
+        <v>39100</v>
+      </c>
+      <c r="G126" t="n">
+        <v>38700</v>
+      </c>
+      <c r="H126" t="n">
+        <v>10</v>
+      </c>
+      <c r="I126" t="n">
+        <v>2</v>
+      </c>
+      <c r="J126" t="n">
+        <v>5</v>
+      </c>
+      <c r="K126" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="n">
+        <v>38900</v>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>LIMIT</t>
+        </is>
+      </c>
+      <c r="C127" t="n">
+        <v>38920</v>
+      </c>
+      <c r="D127" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E127" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F127" t="n">
+        <v>39040</v>
+      </c>
+      <c r="G127" t="n">
+        <v>38900</v>
+      </c>
+      <c r="H127" t="n">
+        <v>10</v>
+      </c>
+      <c r="I127" t="n">
+        <v>2</v>
+      </c>
+      <c r="J127" t="n">
+        <v>5</v>
+      </c>
+      <c r="K127" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="n">
+        <v>38900</v>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>LIMIT</t>
+        </is>
+      </c>
+      <c r="C128" t="n">
+        <v>38920</v>
+      </c>
+      <c r="D128" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E128" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F128" t="n">
+        <v>39040</v>
+      </c>
+      <c r="G128" t="n">
+        <v>38900</v>
+      </c>
+      <c r="H128" t="n">
+        <v>10</v>
+      </c>
+      <c r="I128" t="n">
+        <v>2</v>
+      </c>
+      <c r="J128" t="n">
+        <v>5</v>
+      </c>
+      <c r="K128" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="n">
+        <v>38900</v>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>LIMIT</t>
+        </is>
+      </c>
+      <c r="C129" t="n">
+        <v>38920</v>
+      </c>
+      <c r="D129" t="inlineStr">
+        <is>
+          <t>CE</t>
+        </is>
+      </c>
+      <c r="E129" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F129" t="n">
+        <v>39040</v>
+      </c>
+      <c r="G129" t="n">
+        <v>38900</v>
+      </c>
+      <c r="H129" t="n">
+        <v>10</v>
+      </c>
+      <c r="I129" t="n">
+        <v>2</v>
+      </c>
+      <c r="J129" t="n">
+        <v>5</v>
+      </c>
+      <c r="K129" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="n">
+        <v>38900</v>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>LIMIT</t>
+        </is>
+      </c>
+      <c r="C130" t="n">
+        <v>38920</v>
+      </c>
+      <c r="D130" t="inlineStr">
+        <is>
+          <t>CE</t>
+        </is>
+      </c>
+      <c r="E130" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F130" t="n">
+        <v>39040</v>
+      </c>
+      <c r="G130" t="n">
+        <v>38900</v>
+      </c>
+      <c r="H130" t="n">
+        <v>10</v>
+      </c>
+      <c r="I130" t="n">
+        <v>2</v>
+      </c>
+      <c r="J130" t="n">
+        <v>5</v>
+      </c>
+      <c r="K130" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="n">
+        <v>38900</v>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>LIMIT</t>
+        </is>
+      </c>
+      <c r="C131" t="n">
+        <v>38915</v>
+      </c>
+      <c r="D131" t="inlineStr">
+        <is>
+          <t>CE</t>
+        </is>
+      </c>
+      <c r="E131" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F131" t="n">
+        <v>39020</v>
+      </c>
+      <c r="G131" t="n">
+        <v>38900</v>
+      </c>
+      <c r="H131" t="n">
+        <v>10</v>
+      </c>
+      <c r="I131" t="n">
+        <v>2</v>
+      </c>
+      <c r="J131" t="n">
+        <v>5</v>
+      </c>
+      <c r="K131" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="n">
+        <v>38800</v>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>LIMIT</t>
+        </is>
+      </c>
+      <c r="C132" t="n">
+        <v>39000</v>
+      </c>
+      <c r="D132" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E132" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F132" t="n">
+        <v>39020</v>
+      </c>
+      <c r="G132" t="n">
+        <v>38900</v>
+      </c>
+      <c r="H132" t="n">
+        <v>10</v>
+      </c>
+      <c r="I132" t="n">
+        <v>2</v>
+      </c>
+      <c r="J132" t="n">
+        <v>5</v>
+      </c>
+      <c r="K132" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
one time failed order is being implemented
</commit_message>
<xml_diff>
--- a/storage/Ibkr.xlsx
+++ b/storage/Ibkr.xlsx
@@ -57,11 +57,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -435,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K204"/>
+  <dimension ref="A1:K226"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -444,57 +445,57 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="3" t="inlineStr">
+      <c r="A1" s="4" t="inlineStr">
         <is>
           <t>Trigger_Level_High_Low</t>
         </is>
       </c>
-      <c r="B1" s="3" t="inlineStr">
+      <c r="B1" s="4" t="inlineStr">
         <is>
           <t>Entry_Type</t>
         </is>
       </c>
-      <c r="C1" s="3" t="inlineStr">
+      <c r="C1" s="4" t="inlineStr">
         <is>
           <t>Entry_Strike</t>
         </is>
       </c>
-      <c r="D1" s="3" t="inlineStr">
+      <c r="D1" s="4" t="inlineStr">
         <is>
           <t>Strike_Type</t>
         </is>
       </c>
-      <c r="E1" s="3" t="inlineStr">
+      <c r="E1" s="4" t="inlineStr">
         <is>
           <t>Expiry</t>
         </is>
       </c>
-      <c r="F1" s="3" t="inlineStr">
+      <c r="F1" s="4" t="inlineStr">
         <is>
           <t>Target</t>
         </is>
       </c>
-      <c r="G1" s="3" t="inlineStr">
+      <c r="G1" s="4" t="inlineStr">
         <is>
           <t>Stop_Loss</t>
         </is>
       </c>
-      <c r="H1" s="3" t="inlineStr">
+      <c r="H1" s="4" t="inlineStr">
         <is>
           <t>Qty</t>
         </is>
       </c>
-      <c r="I1" s="3" t="inlineStr">
+      <c r="I1" s="4" t="inlineStr">
         <is>
           <t>Slicing</t>
         </is>
       </c>
-      <c r="J1" s="3" t="inlineStr">
+      <c r="J1" s="4" t="inlineStr">
         <is>
           <t>Time_Interval</t>
         </is>
       </c>
-      <c r="K1" s="3" t="inlineStr">
+      <c r="K1" s="4" t="inlineStr">
         <is>
           <t>Activation</t>
         </is>
@@ -517,7 +518,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E2" s="5" t="n">
+      <c r="E2" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F2" t="n">
@@ -556,7 +557,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E3" s="5" t="n">
+      <c r="E3" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F3" t="n">
@@ -595,7 +596,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E4" s="5" t="n">
+      <c r="E4" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F4" t="n">
@@ -634,7 +635,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E5" s="5" t="n">
+      <c r="E5" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F5" t="n">
@@ -673,7 +674,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E6" s="5" t="n">
+      <c r="E6" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F6" t="n">
@@ -712,7 +713,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E7" s="5" t="n">
+      <c r="E7" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F7" t="n">
@@ -751,7 +752,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E8" s="5" t="n">
+      <c r="E8" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F8" t="n">
@@ -790,7 +791,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E9" s="5" t="n">
+      <c r="E9" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F9" t="n">
@@ -829,7 +830,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E10" s="5" t="n">
+      <c r="E10" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F10" t="n">
@@ -868,7 +869,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E11" s="5" t="n">
+      <c r="E11" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F11" t="n">
@@ -907,7 +908,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E12" s="5" t="n">
+      <c r="E12" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F12" t="n">
@@ -946,7 +947,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E13" s="5" t="n">
+      <c r="E13" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F13" t="n">
@@ -985,7 +986,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E14" s="5" t="n">
+      <c r="E14" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F14" t="n">
@@ -1024,7 +1025,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E15" s="5" t="n">
+      <c r="E15" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F15" t="n">
@@ -1063,7 +1064,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E16" s="5" t="n">
+      <c r="E16" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F16" t="n">
@@ -1102,7 +1103,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E17" s="5" t="n">
+      <c r="E17" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F17" t="n">
@@ -1141,7 +1142,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E18" s="5" t="n">
+      <c r="E18" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F18" t="n">
@@ -1180,7 +1181,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E19" s="5" t="n">
+      <c r="E19" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F19" t="n">
@@ -1219,7 +1220,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E20" s="5" t="n">
+      <c r="E20" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F20" t="n">
@@ -1258,7 +1259,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E21" s="5" t="n">
+      <c r="E21" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F21" t="n">
@@ -1297,7 +1298,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E22" s="5" t="n">
+      <c r="E22" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F22" t="n">
@@ -1336,7 +1337,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E23" s="5" t="n">
+      <c r="E23" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F23" t="n">
@@ -1375,7 +1376,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E24" s="5" t="n">
+      <c r="E24" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F24" t="n">
@@ -1414,7 +1415,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E25" s="5" t="n">
+      <c r="E25" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F25" t="n">
@@ -1453,7 +1454,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E26" s="5" t="n">
+      <c r="E26" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F26" t="n">
@@ -1492,7 +1493,7 @@
           <t>CE</t>
         </is>
       </c>
-      <c r="E27" s="5" t="n">
+      <c r="E27" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F27" t="n">
@@ -1531,7 +1532,7 @@
           <t>CE</t>
         </is>
       </c>
-      <c r="E28" s="5" t="n">
+      <c r="E28" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F28" t="n">
@@ -1570,7 +1571,7 @@
           <t>CE</t>
         </is>
       </c>
-      <c r="E29" s="5" t="n">
+      <c r="E29" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F29" t="n">
@@ -1609,7 +1610,7 @@
           <t>CE</t>
         </is>
       </c>
-      <c r="E30" s="5" t="n">
+      <c r="E30" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F30" t="n">
@@ -1648,7 +1649,7 @@
           <t>CE</t>
         </is>
       </c>
-      <c r="E31" s="5" t="n">
+      <c r="E31" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F31" t="n">
@@ -1687,7 +1688,7 @@
           <t>CE</t>
         </is>
       </c>
-      <c r="E32" s="5" t="n">
+      <c r="E32" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F32" t="n">
@@ -1726,7 +1727,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E33" s="5" t="n">
+      <c r="E33" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F33" t="n">
@@ -1765,7 +1766,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E34" s="5" t="n">
+      <c r="E34" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F34" t="n">
@@ -1804,7 +1805,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E35" s="5" t="n">
+      <c r="E35" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F35" t="n">
@@ -1843,7 +1844,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E36" s="5" t="n">
+      <c r="E36" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F36" t="n">
@@ -1882,7 +1883,7 @@
           <t>CE</t>
         </is>
       </c>
-      <c r="E37" s="5" t="n">
+      <c r="E37" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F37" t="n">
@@ -1921,7 +1922,7 @@
           <t>CE</t>
         </is>
       </c>
-      <c r="E38" s="5" t="n">
+      <c r="E38" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F38" t="n">
@@ -1960,7 +1961,7 @@
           <t>CE</t>
         </is>
       </c>
-      <c r="E39" s="5" t="n">
+      <c r="E39" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F39" t="n">
@@ -1999,7 +2000,7 @@
           <t>CE</t>
         </is>
       </c>
-      <c r="E40" s="5" t="n">
+      <c r="E40" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F40" t="n">
@@ -2038,7 +2039,7 @@
           <t>CE</t>
         </is>
       </c>
-      <c r="E41" s="5" t="n">
+      <c r="E41" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F41" t="n">
@@ -2077,7 +2078,7 @@
           <t>CE</t>
         </is>
       </c>
-      <c r="E42" s="5" t="n">
+      <c r="E42" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F42" t="n">
@@ -2116,7 +2117,7 @@
           <t>CE</t>
         </is>
       </c>
-      <c r="E43" s="5" t="n">
+      <c r="E43" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F43" t="n">
@@ -2155,7 +2156,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E44" s="5" t="n">
+      <c r="E44" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F44" t="n">
@@ -2194,7 +2195,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E45" s="5" t="n">
+      <c r="E45" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F45" t="n">
@@ -2233,7 +2234,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E46" s="5" t="n">
+      <c r="E46" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F46" t="n">
@@ -2272,7 +2273,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E47" s="5" t="n">
+      <c r="E47" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F47" t="n">
@@ -2311,7 +2312,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E48" s="5" t="n">
+      <c r="E48" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F48" t="n">
@@ -2350,7 +2351,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E49" s="5" t="n">
+      <c r="E49" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F49" t="n">
@@ -2389,7 +2390,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E50" s="5" t="n">
+      <c r="E50" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F50" t="n">
@@ -2428,7 +2429,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E51" s="5" t="n">
+      <c r="E51" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F51" t="n">
@@ -2467,7 +2468,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E52" s="5" t="n">
+      <c r="E52" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F52" t="n">
@@ -2506,7 +2507,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E53" s="5" t="n">
+      <c r="E53" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F53" t="n">
@@ -2545,7 +2546,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E54" s="5" t="n">
+      <c r="E54" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F54" t="n">
@@ -2584,7 +2585,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E55" s="5" t="n">
+      <c r="E55" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F55" t="n">
@@ -2623,7 +2624,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E56" s="5" t="n">
+      <c r="E56" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F56" t="n">
@@ -2662,7 +2663,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E57" s="5" t="n">
+      <c r="E57" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F57" t="n">
@@ -2701,7 +2702,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E58" s="5" t="n">
+      <c r="E58" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F58" t="n">
@@ -2740,7 +2741,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E59" s="5" t="n">
+      <c r="E59" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F59" t="n">
@@ -2779,7 +2780,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E60" s="5" t="n">
+      <c r="E60" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F60" t="n">
@@ -2818,7 +2819,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E61" s="5" t="n">
+      <c r="E61" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F61" t="n">
@@ -2857,7 +2858,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E62" s="5" t="n">
+      <c r="E62" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F62" t="n">
@@ -2896,7 +2897,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E63" s="5" t="n">
+      <c r="E63" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F63" t="n">
@@ -2935,7 +2936,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E64" s="5" t="n">
+      <c r="E64" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F64" t="n">
@@ -2974,7 +2975,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E65" s="5" t="n">
+      <c r="E65" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F65" t="n">
@@ -3013,7 +3014,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E66" s="5" t="n">
+      <c r="E66" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F66" t="n">
@@ -3052,7 +3053,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E67" s="5" t="n">
+      <c r="E67" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F67" t="n">
@@ -3091,7 +3092,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E68" s="5" t="n">
+      <c r="E68" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F68" t="n">
@@ -3130,7 +3131,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E69" s="5" t="n">
+      <c r="E69" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F69" t="n">
@@ -3169,7 +3170,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E70" s="5" t="n">
+      <c r="E70" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F70" t="n">
@@ -3208,7 +3209,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E71" s="5" t="n">
+      <c r="E71" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F71" t="n">
@@ -3247,7 +3248,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E72" s="5" t="n">
+      <c r="E72" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F72" t="n">
@@ -3286,7 +3287,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E73" s="5" t="n">
+      <c r="E73" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F73" t="n">
@@ -3325,7 +3326,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E74" s="5" t="n">
+      <c r="E74" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F74" t="n">
@@ -3364,7 +3365,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E75" s="5" t="n">
+      <c r="E75" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F75" t="n">
@@ -3403,7 +3404,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E76" s="5" t="n">
+      <c r="E76" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F76" t="n">
@@ -3442,7 +3443,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E77" s="5" t="n">
+      <c r="E77" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F77" t="n">
@@ -3481,7 +3482,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E78" s="5" t="n">
+      <c r="E78" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F78" t="n">
@@ -3520,7 +3521,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E79" s="5" t="n">
+      <c r="E79" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F79" t="n">
@@ -3559,7 +3560,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E80" s="5" t="n">
+      <c r="E80" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F80" t="n">
@@ -3598,7 +3599,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E81" s="5" t="n">
+      <c r="E81" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F81" t="n">
@@ -3637,7 +3638,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E82" s="5" t="n">
+      <c r="E82" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F82" t="n">
@@ -3676,7 +3677,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E83" s="5" t="n">
+      <c r="E83" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F83" t="n">
@@ -3715,7 +3716,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E84" s="5" t="n">
+      <c r="E84" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F84" t="n">
@@ -3754,7 +3755,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E85" s="5" t="n">
+      <c r="E85" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F85" t="n">
@@ -3793,7 +3794,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E86" s="5" t="n">
+      <c r="E86" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F86" t="n">
@@ -3832,7 +3833,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E87" s="5" t="n">
+      <c r="E87" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F87" t="n">
@@ -3871,7 +3872,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E88" s="5" t="n">
+      <c r="E88" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F88" t="n">
@@ -3910,7 +3911,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E89" s="5" t="n">
+      <c r="E89" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F89" t="n">
@@ -3949,7 +3950,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E90" s="5" t="n">
+      <c r="E90" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F90" t="n">
@@ -3988,7 +3989,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E91" s="5" t="n">
+      <c r="E91" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F91" t="n">
@@ -4027,7 +4028,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E92" s="5" t="n">
+      <c r="E92" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F92" t="n">
@@ -4066,7 +4067,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E93" s="5" t="n">
+      <c r="E93" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F93" t="n">
@@ -4105,7 +4106,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E94" s="5" t="n">
+      <c r="E94" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F94" t="n">
@@ -4144,7 +4145,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E95" s="5" t="n">
+      <c r="E95" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F95" t="n">
@@ -4183,7 +4184,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E96" s="5" t="n">
+      <c r="E96" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F96" t="n">
@@ -4222,7 +4223,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E97" s="5" t="n">
+      <c r="E97" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F97" t="n">
@@ -4261,7 +4262,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E98" s="5" t="n">
+      <c r="E98" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F98" t="n">
@@ -4300,7 +4301,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E99" s="5" t="n">
+      <c r="E99" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F99" t="n">
@@ -4339,7 +4340,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E100" s="5" t="n">
+      <c r="E100" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F100" t="n">
@@ -4378,7 +4379,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E101" s="5" t="n">
+      <c r="E101" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F101" t="n">
@@ -4417,7 +4418,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E102" s="5" t="n">
+      <c r="E102" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F102" t="n">
@@ -4456,7 +4457,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E103" s="5" t="n">
+      <c r="E103" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F103" t="n">
@@ -4495,7 +4496,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E104" s="5" t="n">
+      <c r="E104" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F104" t="n">
@@ -4534,7 +4535,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E105" s="5" t="n">
+      <c r="E105" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F105" t="n">
@@ -4573,7 +4574,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E106" s="5" t="n">
+      <c r="E106" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F106" t="n">
@@ -4612,7 +4613,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E107" s="5" t="n">
+      <c r="E107" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F107" t="n">
@@ -4651,7 +4652,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E108" s="5" t="n">
+      <c r="E108" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F108" t="n">
@@ -4690,7 +4691,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E109" s="5" t="n">
+      <c r="E109" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F109" t="n">
@@ -4729,7 +4730,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E110" s="5" t="n">
+      <c r="E110" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F110" t="n">
@@ -4768,7 +4769,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E111" s="5" t="n">
+      <c r="E111" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F111" t="n">
@@ -4807,7 +4808,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E112" s="5" t="n">
+      <c r="E112" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F112" t="n">
@@ -4846,7 +4847,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E113" s="5" t="n">
+      <c r="E113" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F113" t="n">
@@ -4885,7 +4886,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E114" s="5" t="n">
+      <c r="E114" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F114" t="n">
@@ -4924,7 +4925,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E115" s="5" t="n">
+      <c r="E115" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F115" t="n">
@@ -4963,7 +4964,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E116" s="5" t="n">
+      <c r="E116" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F116" t="n">
@@ -5002,7 +5003,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E117" s="5" t="n">
+      <c r="E117" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F117" t="n">
@@ -5041,7 +5042,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E118" s="5" t="n">
+      <c r="E118" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F118" t="n">
@@ -5080,7 +5081,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E119" s="5" t="n">
+      <c r="E119" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F119" t="n">
@@ -5119,7 +5120,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E120" s="5" t="n">
+      <c r="E120" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F120" t="n">
@@ -5158,7 +5159,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E121" s="5" t="n">
+      <c r="E121" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F121" t="n">
@@ -5197,7 +5198,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E122" s="5" t="n">
+      <c r="E122" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F122" t="n">
@@ -5236,7 +5237,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E123" s="5" t="n">
+      <c r="E123" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F123" t="n">
@@ -5275,7 +5276,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E124" s="5" t="n">
+      <c r="E124" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F124" t="n">
@@ -5314,7 +5315,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E125" s="5" t="n">
+      <c r="E125" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F125" t="n">
@@ -5353,7 +5354,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E126" s="5" t="n">
+      <c r="E126" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F126" t="n">
@@ -5392,7 +5393,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E127" s="5" t="n">
+      <c r="E127" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F127" t="n">
@@ -5431,7 +5432,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E128" s="5" t="n">
+      <c r="E128" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F128" t="n">
@@ -5470,7 +5471,7 @@
           <t>CE</t>
         </is>
       </c>
-      <c r="E129" s="5" t="n">
+      <c r="E129" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F129" t="n">
@@ -5509,7 +5510,7 @@
           <t>CE</t>
         </is>
       </c>
-      <c r="E130" s="5" t="n">
+      <c r="E130" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F130" t="n">
@@ -5548,7 +5549,7 @@
           <t>CE</t>
         </is>
       </c>
-      <c r="E131" s="5" t="n">
+      <c r="E131" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F131" t="n">
@@ -5587,7 +5588,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E132" s="5" t="n">
+      <c r="E132" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F132" t="n">
@@ -5626,7 +5627,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E133" s="5" t="n">
+      <c r="E133" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F133" t="n">
@@ -5665,7 +5666,7 @@
           <t>CE</t>
         </is>
       </c>
-      <c r="E134" s="5" t="n">
+      <c r="E134" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F134" t="n">
@@ -5704,7 +5705,7 @@
           <t>CE</t>
         </is>
       </c>
-      <c r="E135" s="5" t="n">
+      <c r="E135" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F135" t="n">
@@ -5743,7 +5744,7 @@
           <t>CE</t>
         </is>
       </c>
-      <c r="E136" s="5" t="n">
+      <c r="E136" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F136" t="n">
@@ -5782,7 +5783,7 @@
           <t>CE</t>
         </is>
       </c>
-      <c r="E137" s="5" t="n">
+      <c r="E137" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F137" t="n">
@@ -5821,7 +5822,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E138" s="5" t="n">
+      <c r="E138" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F138" t="n">
@@ -5860,7 +5861,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E139" s="5" t="n">
+      <c r="E139" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F139" t="n">
@@ -5899,7 +5900,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E140" s="5" t="n">
+      <c r="E140" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F140" t="n">
@@ -5938,7 +5939,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E141" s="5" t="n">
+      <c r="E141" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F141" t="n">
@@ -5977,7 +5978,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E142" s="5" t="n">
+      <c r="E142" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F142" t="n">
@@ -6016,7 +6017,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E143" s="5" t="n">
+      <c r="E143" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F143" t="n">
@@ -6055,7 +6056,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E144" s="5" t="n">
+      <c r="E144" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F144" t="n">
@@ -6094,7 +6095,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E145" s="5" t="n">
+      <c r="E145" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F145" t="n">
@@ -6133,7 +6134,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E146" s="5" t="n">
+      <c r="E146" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F146" t="n">
@@ -6172,7 +6173,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E147" s="5" t="n">
+      <c r="E147" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F147" t="n">
@@ -6211,7 +6212,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E148" s="5" t="n">
+      <c r="E148" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F148" t="n">
@@ -6250,7 +6251,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E149" s="5" t="n">
+      <c r="E149" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F149" t="n">
@@ -6289,7 +6290,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E150" s="5" t="n">
+      <c r="E150" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F150" t="n">
@@ -6328,7 +6329,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E151" s="5" t="n">
+      <c r="E151" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F151" t="n">
@@ -6367,7 +6368,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E152" s="5" t="n">
+      <c r="E152" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F152" t="n">
@@ -6406,7 +6407,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E153" s="5" t="n">
+      <c r="E153" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F153" t="n">
@@ -6445,7 +6446,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E154" s="5" t="n">
+      <c r="E154" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F154" t="n">
@@ -6484,7 +6485,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E155" s="5" t="n">
+      <c r="E155" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F155" t="n">
@@ -6523,7 +6524,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E156" s="5" t="n">
+      <c r="E156" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F156" t="n">
@@ -6562,7 +6563,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E157" s="5" t="n">
+      <c r="E157" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F157" t="n">
@@ -6601,7 +6602,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E158" s="5" t="n">
+      <c r="E158" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F158" t="n">
@@ -6640,7 +6641,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E159" s="5" t="n">
+      <c r="E159" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F159" t="n">
@@ -6679,7 +6680,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E160" s="5" t="n">
+      <c r="E160" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F160" t="n">
@@ -6718,7 +6719,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E161" s="5" t="n">
+      <c r="E161" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F161" t="n">
@@ -6757,7 +6758,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E162" s="5" t="n">
+      <c r="E162" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F162" t="n">
@@ -6796,7 +6797,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E163" s="5" t="n">
+      <c r="E163" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F163" t="n">
@@ -6835,7 +6836,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E164" s="5" t="n">
+      <c r="E164" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F164" t="n">
@@ -6874,7 +6875,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E165" s="5" t="n">
+      <c r="E165" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F165" t="n">
@@ -6913,7 +6914,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E166" s="5" t="n">
+      <c r="E166" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F166" t="n">
@@ -6952,7 +6953,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E167" s="5" t="n">
+      <c r="E167" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F167" t="n">
@@ -6991,7 +6992,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E168" s="5" t="n">
+      <c r="E168" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F168" t="n">
@@ -7030,7 +7031,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E169" s="5" t="n">
+      <c r="E169" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F169" t="n">
@@ -7069,7 +7070,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E170" s="5" t="n">
+      <c r="E170" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F170" t="n">
@@ -7108,7 +7109,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E171" s="5" t="n">
+      <c r="E171" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F171" t="n">
@@ -7147,7 +7148,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E172" s="5" t="n">
+      <c r="E172" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F172" t="n">
@@ -7186,7 +7187,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E173" s="5" t="n">
+      <c r="E173" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F173" t="n">
@@ -7225,7 +7226,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E174" s="5" t="n">
+      <c r="E174" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F174" t="n">
@@ -7264,7 +7265,7 @@
           <t>CE</t>
         </is>
       </c>
-      <c r="E175" s="5" t="n">
+      <c r="E175" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F175" t="n">
@@ -7303,7 +7304,7 @@
           <t>CE</t>
         </is>
       </c>
-      <c r="E176" s="5" t="n">
+      <c r="E176" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F176" t="n">
@@ -7342,7 +7343,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E177" s="5" t="n">
+      <c r="E177" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F177" t="n">
@@ -7381,7 +7382,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E178" s="5" t="n">
+      <c r="E178" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F178" t="n">
@@ -7420,7 +7421,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E179" s="5" t="n">
+      <c r="E179" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F179" t="n">
@@ -7459,7 +7460,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E180" s="5" t="n">
+      <c r="E180" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F180" t="n">
@@ -7498,7 +7499,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E181" s="5" t="n">
+      <c r="E181" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F181" t="n">
@@ -7537,7 +7538,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E182" s="5" t="n">
+      <c r="E182" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F182" t="n">
@@ -7576,7 +7577,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E183" s="5" t="n">
+      <c r="E183" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F183" t="n">
@@ -7615,7 +7616,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E184" s="5" t="n">
+      <c r="E184" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F184" t="n">
@@ -7654,7 +7655,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E185" s="5" t="n">
+      <c r="E185" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F185" t="n">
@@ -7693,7 +7694,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E186" s="5" t="n">
+      <c r="E186" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F186" t="n">
@@ -7732,7 +7733,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E187" s="5" t="n">
+      <c r="E187" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F187" t="n">
@@ -7771,7 +7772,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E188" s="5" t="n">
+      <c r="E188" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F188" t="n">
@@ -7810,7 +7811,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E189" s="5" t="n">
+      <c r="E189" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F189" t="n">
@@ -7849,7 +7850,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E190" s="5" t="n">
+      <c r="E190" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F190" t="n">
@@ -7888,7 +7889,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E191" s="5" t="n">
+      <c r="E191" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F191" t="n">
@@ -7927,7 +7928,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E192" s="5" t="n">
+      <c r="E192" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F192" t="n">
@@ -7966,7 +7967,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E193" s="5" t="n">
+      <c r="E193" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F193" t="n">
@@ -8005,7 +8006,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E194" s="5" t="n">
+      <c r="E194" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F194" t="n">
@@ -8044,7 +8045,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E195" s="5" t="n">
+      <c r="E195" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F195" t="n">
@@ -8083,7 +8084,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E196" s="5" t="n">
+      <c r="E196" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F196" t="n">
@@ -8122,7 +8123,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E197" s="5" t="n">
+      <c r="E197" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F197" t="n">
@@ -8161,7 +8162,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E198" s="5" t="n">
+      <c r="E198" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F198" t="n">
@@ -8200,7 +8201,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E199" s="5" t="n">
+      <c r="E199" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F199" t="n">
@@ -8239,7 +8240,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E200" s="5" t="n">
+      <c r="E200" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F200" t="n">
@@ -8278,7 +8279,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E201" s="5" t="n">
+      <c r="E201" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F201" t="n">
@@ -8317,7 +8318,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E202" s="5" t="n">
+      <c r="E202" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F202" t="n">
@@ -8356,7 +8357,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E203" s="5" t="n">
+      <c r="E203" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F203" t="n">
@@ -8395,7 +8396,7 @@
           <t>PE</t>
         </is>
       </c>
-      <c r="E204" s="5" t="n">
+      <c r="E204" s="6" t="n">
         <v>45660</v>
       </c>
       <c r="F204" t="n">
@@ -8414,6 +8415,864 @@
         <v>5</v>
       </c>
       <c r="K204" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="n">
+        <v>39250</v>
+      </c>
+      <c r="B205" t="inlineStr">
+        <is>
+          <t>LIMIT</t>
+        </is>
+      </c>
+      <c r="C205" t="n">
+        <v>39400</v>
+      </c>
+      <c r="D205" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E205" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F205" t="n">
+        <v>39500</v>
+      </c>
+      <c r="G205" t="n">
+        <v>39300</v>
+      </c>
+      <c r="H205" t="n">
+        <v>4</v>
+      </c>
+      <c r="I205" t="n">
+        <v>2</v>
+      </c>
+      <c r="J205" t="n">
+        <v>5</v>
+      </c>
+      <c r="K205" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="n">
+        <v>39250</v>
+      </c>
+      <c r="B206" t="inlineStr">
+        <is>
+          <t>LIMIT</t>
+        </is>
+      </c>
+      <c r="C206" t="n">
+        <v>39400</v>
+      </c>
+      <c r="D206" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E206" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F206" t="n">
+        <v>39500</v>
+      </c>
+      <c r="G206" t="n">
+        <v>39300</v>
+      </c>
+      <c r="H206" t="n">
+        <v>4</v>
+      </c>
+      <c r="I206" t="n">
+        <v>2</v>
+      </c>
+      <c r="J206" t="n">
+        <v>5</v>
+      </c>
+      <c r="K206" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="n">
+        <v>39250</v>
+      </c>
+      <c r="B207" t="inlineStr">
+        <is>
+          <t>LIMIT</t>
+        </is>
+      </c>
+      <c r="C207" t="n">
+        <v>39400</v>
+      </c>
+      <c r="D207" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E207" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F207" t="n">
+        <v>39500</v>
+      </c>
+      <c r="G207" t="n">
+        <v>39300</v>
+      </c>
+      <c r="H207" t="n">
+        <v>4</v>
+      </c>
+      <c r="I207" t="n">
+        <v>2</v>
+      </c>
+      <c r="J207" t="n">
+        <v>5</v>
+      </c>
+      <c r="K207" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="n">
+        <v>39250</v>
+      </c>
+      <c r="B208" t="inlineStr">
+        <is>
+          <t>LIMIT</t>
+        </is>
+      </c>
+      <c r="C208" t="n">
+        <v>39400</v>
+      </c>
+      <c r="D208" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E208" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F208" t="n">
+        <v>39500</v>
+      </c>
+      <c r="G208" t="n">
+        <v>39300</v>
+      </c>
+      <c r="H208" t="n">
+        <v>4</v>
+      </c>
+      <c r="I208" t="n">
+        <v>2</v>
+      </c>
+      <c r="J208" t="n">
+        <v>5</v>
+      </c>
+      <c r="K208" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="n">
+        <v>39250</v>
+      </c>
+      <c r="B209" t="inlineStr">
+        <is>
+          <t>LIMIT</t>
+        </is>
+      </c>
+      <c r="C209" t="n">
+        <v>39400</v>
+      </c>
+      <c r="D209" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E209" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F209" t="n">
+        <v>39500</v>
+      </c>
+      <c r="G209" t="n">
+        <v>39300</v>
+      </c>
+      <c r="H209" t="n">
+        <v>4</v>
+      </c>
+      <c r="I209" t="n">
+        <v>2</v>
+      </c>
+      <c r="J209" t="n">
+        <v>5</v>
+      </c>
+      <c r="K209" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="n">
+        <v>39250</v>
+      </c>
+      <c r="B210" t="inlineStr">
+        <is>
+          <t>LIMIT</t>
+        </is>
+      </c>
+      <c r="C210" t="n">
+        <v>39400</v>
+      </c>
+      <c r="D210" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E210" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F210" t="n">
+        <v>39500</v>
+      </c>
+      <c r="G210" t="n">
+        <v>39300</v>
+      </c>
+      <c r="H210" t="n">
+        <v>4</v>
+      </c>
+      <c r="I210" t="n">
+        <v>2</v>
+      </c>
+      <c r="J210" t="n">
+        <v>5</v>
+      </c>
+      <c r="K210" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="n">
+        <v>39250</v>
+      </c>
+      <c r="B211" t="inlineStr">
+        <is>
+          <t>LIMIT</t>
+        </is>
+      </c>
+      <c r="C211" t="n">
+        <v>39400</v>
+      </c>
+      <c r="D211" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E211" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F211" t="n">
+        <v>39500</v>
+      </c>
+      <c r="G211" t="n">
+        <v>39300</v>
+      </c>
+      <c r="H211" t="n">
+        <v>4</v>
+      </c>
+      <c r="I211" t="n">
+        <v>2</v>
+      </c>
+      <c r="J211" t="n">
+        <v>5</v>
+      </c>
+      <c r="K211" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="n">
+        <v>39250</v>
+      </c>
+      <c r="B212" t="inlineStr">
+        <is>
+          <t>LIMIT</t>
+        </is>
+      </c>
+      <c r="C212" t="n">
+        <v>39400</v>
+      </c>
+      <c r="D212" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E212" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F212" t="n">
+        <v>39500</v>
+      </c>
+      <c r="G212" t="n">
+        <v>39300</v>
+      </c>
+      <c r="H212" t="n">
+        <v>4</v>
+      </c>
+      <c r="I212" t="n">
+        <v>2</v>
+      </c>
+      <c r="J212" t="n">
+        <v>5</v>
+      </c>
+      <c r="K212" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="n">
+        <v>39250</v>
+      </c>
+      <c r="B213" t="inlineStr">
+        <is>
+          <t>LIMIT</t>
+        </is>
+      </c>
+      <c r="C213" t="n">
+        <v>39400</v>
+      </c>
+      <c r="D213" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E213" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F213" t="n">
+        <v>39500</v>
+      </c>
+      <c r="G213" t="n">
+        <v>39300</v>
+      </c>
+      <c r="H213" t="n">
+        <v>4</v>
+      </c>
+      <c r="I213" t="n">
+        <v>2</v>
+      </c>
+      <c r="J213" t="n">
+        <v>5</v>
+      </c>
+      <c r="K213" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="n">
+        <v>39250</v>
+      </c>
+      <c r="B214" t="inlineStr">
+        <is>
+          <t>LIMIT</t>
+        </is>
+      </c>
+      <c r="C214" t="n">
+        <v>39400</v>
+      </c>
+      <c r="D214" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E214" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F214" t="n">
+        <v>39500</v>
+      </c>
+      <c r="G214" t="n">
+        <v>39300</v>
+      </c>
+      <c r="H214" t="n">
+        <v>4</v>
+      </c>
+      <c r="I214" t="n">
+        <v>2</v>
+      </c>
+      <c r="J214" t="n">
+        <v>5</v>
+      </c>
+      <c r="K214" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="n">
+        <v>39250</v>
+      </c>
+      <c r="B215" t="inlineStr">
+        <is>
+          <t>LIMIT</t>
+        </is>
+      </c>
+      <c r="C215" t="n">
+        <v>39400</v>
+      </c>
+      <c r="D215" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E215" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F215" t="n">
+        <v>39500</v>
+      </c>
+      <c r="G215" t="n">
+        <v>39300</v>
+      </c>
+      <c r="H215" t="n">
+        <v>4</v>
+      </c>
+      <c r="I215" t="n">
+        <v>2</v>
+      </c>
+      <c r="J215" t="n">
+        <v>5</v>
+      </c>
+      <c r="K215" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="n">
+        <v>39250</v>
+      </c>
+      <c r="B216" t="inlineStr">
+        <is>
+          <t>LIMIT</t>
+        </is>
+      </c>
+      <c r="C216" t="n">
+        <v>39400</v>
+      </c>
+      <c r="D216" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E216" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F216" t="n">
+        <v>39500</v>
+      </c>
+      <c r="G216" t="n">
+        <v>39300</v>
+      </c>
+      <c r="H216" t="n">
+        <v>4</v>
+      </c>
+      <c r="I216" t="n">
+        <v>2</v>
+      </c>
+      <c r="J216" t="n">
+        <v>5</v>
+      </c>
+      <c r="K216" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="n">
+        <v>39250</v>
+      </c>
+      <c r="B217" t="inlineStr">
+        <is>
+          <t>LIMIT</t>
+        </is>
+      </c>
+      <c r="C217" t="n">
+        <v>39400</v>
+      </c>
+      <c r="D217" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E217" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F217" t="n">
+        <v>39500</v>
+      </c>
+      <c r="G217" t="n">
+        <v>39300</v>
+      </c>
+      <c r="H217" t="n">
+        <v>4</v>
+      </c>
+      <c r="I217" t="n">
+        <v>2</v>
+      </c>
+      <c r="J217" t="n">
+        <v>5</v>
+      </c>
+      <c r="K217" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="n">
+        <v>39250</v>
+      </c>
+      <c r="B218" t="inlineStr">
+        <is>
+          <t>LIMIT</t>
+        </is>
+      </c>
+      <c r="C218" t="n">
+        <v>39400</v>
+      </c>
+      <c r="D218" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E218" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F218" t="n">
+        <v>39500</v>
+      </c>
+      <c r="G218" t="n">
+        <v>39300</v>
+      </c>
+      <c r="H218" t="n">
+        <v>4</v>
+      </c>
+      <c r="I218" t="n">
+        <v>2</v>
+      </c>
+      <c r="J218" t="n">
+        <v>5</v>
+      </c>
+      <c r="K218" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="n">
+        <v>39250</v>
+      </c>
+      <c r="B219" t="inlineStr">
+        <is>
+          <t>LIMIT</t>
+        </is>
+      </c>
+      <c r="C219" t="n">
+        <v>39400</v>
+      </c>
+      <c r="D219" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E219" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F219" t="n">
+        <v>39500</v>
+      </c>
+      <c r="G219" t="n">
+        <v>39300</v>
+      </c>
+      <c r="H219" t="n">
+        <v>4</v>
+      </c>
+      <c r="I219" t="n">
+        <v>2</v>
+      </c>
+      <c r="J219" t="n">
+        <v>5</v>
+      </c>
+      <c r="K219" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="n">
+        <v>39250</v>
+      </c>
+      <c r="B220" t="inlineStr">
+        <is>
+          <t>LIMIT</t>
+        </is>
+      </c>
+      <c r="C220" t="n">
+        <v>39400</v>
+      </c>
+      <c r="D220" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E220" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F220" t="n">
+        <v>39500</v>
+      </c>
+      <c r="G220" t="n">
+        <v>39300</v>
+      </c>
+      <c r="H220" t="n">
+        <v>4</v>
+      </c>
+      <c r="I220" t="n">
+        <v>2</v>
+      </c>
+      <c r="J220" t="n">
+        <v>5</v>
+      </c>
+      <c r="K220" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="n">
+        <v>39250</v>
+      </c>
+      <c r="B221" t="inlineStr">
+        <is>
+          <t>LIMIT</t>
+        </is>
+      </c>
+      <c r="C221" t="n">
+        <v>39400</v>
+      </c>
+      <c r="D221" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E221" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F221" t="n">
+        <v>39500</v>
+      </c>
+      <c r="G221" t="n">
+        <v>39300</v>
+      </c>
+      <c r="H221" t="n">
+        <v>4</v>
+      </c>
+      <c r="I221" t="n">
+        <v>2</v>
+      </c>
+      <c r="J221" t="n">
+        <v>5</v>
+      </c>
+      <c r="K221" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="n">
+        <v>39250</v>
+      </c>
+      <c r="B222" t="inlineStr">
+        <is>
+          <t>LIMIT</t>
+        </is>
+      </c>
+      <c r="C222" t="n">
+        <v>39400</v>
+      </c>
+      <c r="D222" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E222" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F222" t="n">
+        <v>39500</v>
+      </c>
+      <c r="G222" t="n">
+        <v>39300</v>
+      </c>
+      <c r="H222" t="n">
+        <v>4</v>
+      </c>
+      <c r="I222" t="n">
+        <v>2</v>
+      </c>
+      <c r="J222" t="n">
+        <v>5</v>
+      </c>
+      <c r="K222" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="n">
+        <v>39250</v>
+      </c>
+      <c r="B223" t="inlineStr">
+        <is>
+          <t>LIMIT</t>
+        </is>
+      </c>
+      <c r="C223" t="n">
+        <v>39400</v>
+      </c>
+      <c r="D223" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E223" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F223" t="n">
+        <v>39500</v>
+      </c>
+      <c r="G223" t="n">
+        <v>39300</v>
+      </c>
+      <c r="H223" t="n">
+        <v>4</v>
+      </c>
+      <c r="I223" t="n">
+        <v>2</v>
+      </c>
+      <c r="J223" t="n">
+        <v>5</v>
+      </c>
+      <c r="K223" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="n">
+        <v>39250</v>
+      </c>
+      <c r="B224" t="inlineStr">
+        <is>
+          <t>LIMIT</t>
+        </is>
+      </c>
+      <c r="C224" t="n">
+        <v>39400</v>
+      </c>
+      <c r="D224" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E224" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F224" t="n">
+        <v>39500</v>
+      </c>
+      <c r="G224" t="n">
+        <v>39300</v>
+      </c>
+      <c r="H224" t="n">
+        <v>4</v>
+      </c>
+      <c r="I224" t="n">
+        <v>2</v>
+      </c>
+      <c r="J224" t="n">
+        <v>5</v>
+      </c>
+      <c r="K224" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="n">
+        <v>39250</v>
+      </c>
+      <c r="B225" t="inlineStr">
+        <is>
+          <t>LIMIT</t>
+        </is>
+      </c>
+      <c r="C225" t="n">
+        <v>39400</v>
+      </c>
+      <c r="D225" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E225" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F225" t="n">
+        <v>39500</v>
+      </c>
+      <c r="G225" t="n">
+        <v>39300</v>
+      </c>
+      <c r="H225" t="n">
+        <v>4</v>
+      </c>
+      <c r="I225" t="n">
+        <v>2</v>
+      </c>
+      <c r="J225" t="n">
+        <v>5</v>
+      </c>
+      <c r="K225" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="n">
+        <v>39250</v>
+      </c>
+      <c r="B226" t="inlineStr">
+        <is>
+          <t>LIMIT</t>
+        </is>
+      </c>
+      <c r="C226" t="n">
+        <v>39400</v>
+      </c>
+      <c r="D226" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E226" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F226" t="n">
+        <v>39500</v>
+      </c>
+      <c r="G226" t="n">
+        <v>39300</v>
+      </c>
+      <c r="H226" t="n">
+        <v>4</v>
+      </c>
+      <c r="I226" t="n">
+        <v>2</v>
+      </c>
+      <c r="J226" t="n">
+        <v>5</v>
+      </c>
+      <c r="K226" t="n">
         <v>-1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
three order loop added
</commit_message>
<xml_diff>
--- a/storage/Ibkr.xlsx
+++ b/storage/Ibkr.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K226"/>
+  <dimension ref="A1:K249"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9273,7 +9273,904 @@
         <v>5</v>
       </c>
       <c r="K226" t="n">
-        <v>-1</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="n">
+        <v>39250</v>
+      </c>
+      <c r="B227" t="inlineStr">
+        <is>
+          <t>LIMIT</t>
+        </is>
+      </c>
+      <c r="C227" t="n">
+        <v>39400</v>
+      </c>
+      <c r="D227" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E227" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F227" t="n">
+        <v>39500</v>
+      </c>
+      <c r="G227" t="n">
+        <v>39300</v>
+      </c>
+      <c r="H227" t="n">
+        <v>4</v>
+      </c>
+      <c r="I227" t="n">
+        <v>2</v>
+      </c>
+      <c r="J227" t="n">
+        <v>5</v>
+      </c>
+      <c r="K227" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="n">
+        <v>39250</v>
+      </c>
+      <c r="B228" t="inlineStr">
+        <is>
+          <t>LIMIT</t>
+        </is>
+      </c>
+      <c r="C228" t="n">
+        <v>39400</v>
+      </c>
+      <c r="D228" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E228" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F228" t="n">
+        <v>39500</v>
+      </c>
+      <c r="G228" t="n">
+        <v>39300</v>
+      </c>
+      <c r="H228" t="n">
+        <v>4</v>
+      </c>
+      <c r="I228" t="n">
+        <v>2</v>
+      </c>
+      <c r="J228" t="n">
+        <v>5</v>
+      </c>
+      <c r="K228" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="n">
+        <v>39250</v>
+      </c>
+      <c r="B229" t="inlineStr">
+        <is>
+          <t>LIMIT</t>
+        </is>
+      </c>
+      <c r="C229" t="n">
+        <v>39400</v>
+      </c>
+      <c r="D229" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E229" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F229" t="n">
+        <v>39500</v>
+      </c>
+      <c r="G229" t="n">
+        <v>39300</v>
+      </c>
+      <c r="H229" t="n">
+        <v>4</v>
+      </c>
+      <c r="I229" t="n">
+        <v>2</v>
+      </c>
+      <c r="J229" t="n">
+        <v>5</v>
+      </c>
+      <c r="K229" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="n">
+        <v>39250</v>
+      </c>
+      <c r="B230" t="inlineStr">
+        <is>
+          <t>LIMIT</t>
+        </is>
+      </c>
+      <c r="C230" t="n">
+        <v>39400</v>
+      </c>
+      <c r="D230" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E230" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F230" t="n">
+        <v>39500</v>
+      </c>
+      <c r="G230" t="n">
+        <v>39300</v>
+      </c>
+      <c r="H230" t="n">
+        <v>4</v>
+      </c>
+      <c r="I230" t="n">
+        <v>2</v>
+      </c>
+      <c r="J230" t="n">
+        <v>5</v>
+      </c>
+      <c r="K230" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="n">
+        <v>39250</v>
+      </c>
+      <c r="B231" t="inlineStr">
+        <is>
+          <t>LIMIT</t>
+        </is>
+      </c>
+      <c r="C231" t="n">
+        <v>39400</v>
+      </c>
+      <c r="D231" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E231" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F231" t="n">
+        <v>39500</v>
+      </c>
+      <c r="G231" t="n">
+        <v>39300</v>
+      </c>
+      <c r="H231" t="n">
+        <v>4</v>
+      </c>
+      <c r="I231" t="n">
+        <v>2</v>
+      </c>
+      <c r="J231" t="n">
+        <v>5</v>
+      </c>
+      <c r="K231" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="n">
+        <v>39250</v>
+      </c>
+      <c r="B232" t="inlineStr">
+        <is>
+          <t>LIMIT</t>
+        </is>
+      </c>
+      <c r="C232" t="n">
+        <v>39400</v>
+      </c>
+      <c r="D232" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E232" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F232" t="n">
+        <v>39500</v>
+      </c>
+      <c r="G232" t="n">
+        <v>39300</v>
+      </c>
+      <c r="H232" t="n">
+        <v>4</v>
+      </c>
+      <c r="I232" t="n">
+        <v>2</v>
+      </c>
+      <c r="J232" t="n">
+        <v>5</v>
+      </c>
+      <c r="K232" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="n">
+        <v>39250</v>
+      </c>
+      <c r="B233" t="inlineStr">
+        <is>
+          <t>LIMIT</t>
+        </is>
+      </c>
+      <c r="C233" t="n">
+        <v>39400</v>
+      </c>
+      <c r="D233" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E233" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F233" t="n">
+        <v>39500</v>
+      </c>
+      <c r="G233" t="n">
+        <v>39300</v>
+      </c>
+      <c r="H233" t="n">
+        <v>4</v>
+      </c>
+      <c r="I233" t="n">
+        <v>2</v>
+      </c>
+      <c r="J233" t="n">
+        <v>5</v>
+      </c>
+      <c r="K233" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="n">
+        <v>39250</v>
+      </c>
+      <c r="B234" t="inlineStr">
+        <is>
+          <t>LIMIT</t>
+        </is>
+      </c>
+      <c r="C234" t="n">
+        <v>39400</v>
+      </c>
+      <c r="D234" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E234" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F234" t="n">
+        <v>39500</v>
+      </c>
+      <c r="G234" t="n">
+        <v>39300</v>
+      </c>
+      <c r="H234" t="n">
+        <v>4</v>
+      </c>
+      <c r="I234" t="n">
+        <v>2</v>
+      </c>
+      <c r="J234" t="n">
+        <v>5</v>
+      </c>
+      <c r="K234" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="n">
+        <v>39250</v>
+      </c>
+      <c r="B235" t="inlineStr">
+        <is>
+          <t>LIMIT</t>
+        </is>
+      </c>
+      <c r="C235" t="n">
+        <v>39400</v>
+      </c>
+      <c r="D235" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E235" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F235" t="n">
+        <v>39500</v>
+      </c>
+      <c r="G235" t="n">
+        <v>39300</v>
+      </c>
+      <c r="H235" t="n">
+        <v>4</v>
+      </c>
+      <c r="I235" t="n">
+        <v>2</v>
+      </c>
+      <c r="J235" t="n">
+        <v>5</v>
+      </c>
+      <c r="K235" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="n">
+        <v>39250</v>
+      </c>
+      <c r="B236" t="inlineStr">
+        <is>
+          <t>LIMIT</t>
+        </is>
+      </c>
+      <c r="C236" t="n">
+        <v>39400</v>
+      </c>
+      <c r="D236" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E236" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F236" t="n">
+        <v>39500</v>
+      </c>
+      <c r="G236" t="n">
+        <v>39300</v>
+      </c>
+      <c r="H236" t="n">
+        <v>4</v>
+      </c>
+      <c r="I236" t="n">
+        <v>2</v>
+      </c>
+      <c r="J236" t="n">
+        <v>5</v>
+      </c>
+      <c r="K236" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="n">
+        <v>39250</v>
+      </c>
+      <c r="B237" t="inlineStr">
+        <is>
+          <t>LIMIT</t>
+        </is>
+      </c>
+      <c r="C237" t="n">
+        <v>39400</v>
+      </c>
+      <c r="D237" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E237" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F237" t="n">
+        <v>39500</v>
+      </c>
+      <c r="G237" t="n">
+        <v>39300</v>
+      </c>
+      <c r="H237" t="n">
+        <v>4</v>
+      </c>
+      <c r="I237" t="n">
+        <v>2</v>
+      </c>
+      <c r="J237" t="n">
+        <v>5</v>
+      </c>
+      <c r="K237" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="n">
+        <v>39250</v>
+      </c>
+      <c r="B238" t="inlineStr">
+        <is>
+          <t>LIMIT</t>
+        </is>
+      </c>
+      <c r="C238" t="n">
+        <v>39400</v>
+      </c>
+      <c r="D238" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E238" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F238" t="n">
+        <v>39500</v>
+      </c>
+      <c r="G238" t="n">
+        <v>39300</v>
+      </c>
+      <c r="H238" t="n">
+        <v>4</v>
+      </c>
+      <c r="I238" t="n">
+        <v>2</v>
+      </c>
+      <c r="J238" t="n">
+        <v>5</v>
+      </c>
+      <c r="K238" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="n">
+        <v>39250</v>
+      </c>
+      <c r="B239" t="inlineStr">
+        <is>
+          <t>LIMIT</t>
+        </is>
+      </c>
+      <c r="C239" t="n">
+        <v>39400</v>
+      </c>
+      <c r="D239" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E239" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F239" t="n">
+        <v>39500</v>
+      </c>
+      <c r="G239" t="n">
+        <v>39300</v>
+      </c>
+      <c r="H239" t="n">
+        <v>4</v>
+      </c>
+      <c r="I239" t="n">
+        <v>2</v>
+      </c>
+      <c r="J239" t="n">
+        <v>5</v>
+      </c>
+      <c r="K239" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="n">
+        <v>39250</v>
+      </c>
+      <c r="B240" t="inlineStr">
+        <is>
+          <t>LIMIT</t>
+        </is>
+      </c>
+      <c r="C240" t="n">
+        <v>39400</v>
+      </c>
+      <c r="D240" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E240" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F240" t="n">
+        <v>39500</v>
+      </c>
+      <c r="G240" t="n">
+        <v>39300</v>
+      </c>
+      <c r="H240" t="n">
+        <v>4</v>
+      </c>
+      <c r="I240" t="n">
+        <v>2</v>
+      </c>
+      <c r="J240" t="n">
+        <v>5</v>
+      </c>
+      <c r="K240" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="n">
+        <v>39250</v>
+      </c>
+      <c r="B241" t="inlineStr">
+        <is>
+          <t>LIMIT</t>
+        </is>
+      </c>
+      <c r="C241" t="n">
+        <v>39400</v>
+      </c>
+      <c r="D241" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E241" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F241" t="n">
+        <v>39500</v>
+      </c>
+      <c r="G241" t="n">
+        <v>39300</v>
+      </c>
+      <c r="H241" t="n">
+        <v>4</v>
+      </c>
+      <c r="I241" t="n">
+        <v>2</v>
+      </c>
+      <c r="J241" t="n">
+        <v>5</v>
+      </c>
+      <c r="K241" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="n">
+        <v>39250</v>
+      </c>
+      <c r="B242" t="inlineStr">
+        <is>
+          <t>MARKET</t>
+        </is>
+      </c>
+      <c r="C242" t="n">
+        <v>39400</v>
+      </c>
+      <c r="D242" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E242" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F242" t="n">
+        <v>39500</v>
+      </c>
+      <c r="G242" t="n">
+        <v>39300</v>
+      </c>
+      <c r="H242" t="n">
+        <v>4</v>
+      </c>
+      <c r="I242" t="n">
+        <v>2</v>
+      </c>
+      <c r="J242" t="n">
+        <v>5</v>
+      </c>
+      <c r="K242" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" t="n">
+        <v>39250</v>
+      </c>
+      <c r="B243" t="inlineStr">
+        <is>
+          <t>MARKET</t>
+        </is>
+      </c>
+      <c r="C243" t="n">
+        <v>39400</v>
+      </c>
+      <c r="D243" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E243" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F243" t="n">
+        <v>39500</v>
+      </c>
+      <c r="G243" t="n">
+        <v>39300</v>
+      </c>
+      <c r="H243" t="n">
+        <v>4</v>
+      </c>
+      <c r="I243" t="n">
+        <v>2</v>
+      </c>
+      <c r="J243" t="n">
+        <v>5</v>
+      </c>
+      <c r="K243" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="n">
+        <v>39250</v>
+      </c>
+      <c r="B244" t="inlineStr">
+        <is>
+          <t>MARKET</t>
+        </is>
+      </c>
+      <c r="C244" t="n">
+        <v>39400</v>
+      </c>
+      <c r="D244" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E244" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F244" t="n">
+        <v>39500</v>
+      </c>
+      <c r="G244" t="n">
+        <v>39300</v>
+      </c>
+      <c r="H244" t="n">
+        <v>4</v>
+      </c>
+      <c r="I244" t="n">
+        <v>2</v>
+      </c>
+      <c r="J244" t="n">
+        <v>5</v>
+      </c>
+      <c r="K244" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="n">
+        <v>39250</v>
+      </c>
+      <c r="B245" t="inlineStr">
+        <is>
+          <t>MARKET</t>
+        </is>
+      </c>
+      <c r="C245" t="n">
+        <v>39400</v>
+      </c>
+      <c r="D245" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E245" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F245" t="n">
+        <v>39500</v>
+      </c>
+      <c r="G245" t="n">
+        <v>39300</v>
+      </c>
+      <c r="H245" t="n">
+        <v>4</v>
+      </c>
+      <c r="I245" t="n">
+        <v>2</v>
+      </c>
+      <c r="J245" t="n">
+        <v>5</v>
+      </c>
+      <c r="K245" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="n">
+        <v>39250</v>
+      </c>
+      <c r="B246" t="inlineStr">
+        <is>
+          <t>MARKET</t>
+        </is>
+      </c>
+      <c r="C246" t="n">
+        <v>39400</v>
+      </c>
+      <c r="D246" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E246" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F246" t="n">
+        <v>39500</v>
+      </c>
+      <c r="G246" t="n">
+        <v>39300</v>
+      </c>
+      <c r="H246" t="n">
+        <v>4</v>
+      </c>
+      <c r="I246" t="n">
+        <v>2</v>
+      </c>
+      <c r="J246" t="n">
+        <v>5</v>
+      </c>
+      <c r="K246" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="n">
+        <v>39250</v>
+      </c>
+      <c r="B247" t="inlineStr">
+        <is>
+          <t>MARKET</t>
+        </is>
+      </c>
+      <c r="C247" t="n">
+        <v>39400</v>
+      </c>
+      <c r="D247" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E247" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F247" t="n">
+        <v>39500</v>
+      </c>
+      <c r="G247" t="n">
+        <v>39300</v>
+      </c>
+      <c r="H247" t="n">
+        <v>4</v>
+      </c>
+      <c r="I247" t="n">
+        <v>2</v>
+      </c>
+      <c r="J247" t="n">
+        <v>5</v>
+      </c>
+      <c r="K247" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="n">
+        <v>39250</v>
+      </c>
+      <c r="B248" t="inlineStr">
+        <is>
+          <t>MARKET</t>
+        </is>
+      </c>
+      <c r="C248" t="n">
+        <v>39400</v>
+      </c>
+      <c r="D248" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E248" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F248" t="n">
+        <v>39500</v>
+      </c>
+      <c r="G248" t="n">
+        <v>39300</v>
+      </c>
+      <c r="H248" t="n">
+        <v>4</v>
+      </c>
+      <c r="I248" t="n">
+        <v>2</v>
+      </c>
+      <c r="J248" t="n">
+        <v>5</v>
+      </c>
+      <c r="K248" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="n">
+        <v>39250</v>
+      </c>
+      <c r="B249" t="inlineStr">
+        <is>
+          <t>MARKET</t>
+        </is>
+      </c>
+      <c r="C249" t="n">
+        <v>39400</v>
+      </c>
+      <c r="D249" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E249" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F249" t="n">
+        <v>39500</v>
+      </c>
+      <c r="G249" t="n">
+        <v>39300</v>
+      </c>
+      <c r="H249" t="n">
+        <v>4</v>
+      </c>
+      <c r="I249" t="n">
+        <v>2</v>
+      </c>
+      <c r="J249" t="n">
+        <v>5</v>
+      </c>
+      <c r="K249" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
three times order fixed and working only market_data subscription left and variables left
</commit_message>
<xml_diff>
--- a/storage/Ibkr.xlsx
+++ b/storage/Ibkr.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K249"/>
+  <dimension ref="A1:K268"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10170,7 +10170,748 @@
         <v>5</v>
       </c>
       <c r="K249" t="n">
-        <v>1</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="n">
+        <v>39250</v>
+      </c>
+      <c r="B250" t="inlineStr">
+        <is>
+          <t>MARKET</t>
+        </is>
+      </c>
+      <c r="C250" t="n">
+        <v>39400</v>
+      </c>
+      <c r="D250" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E250" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F250" t="n">
+        <v>39500</v>
+      </c>
+      <c r="G250" t="n">
+        <v>39300</v>
+      </c>
+      <c r="H250" t="n">
+        <v>4</v>
+      </c>
+      <c r="I250" t="n">
+        <v>2</v>
+      </c>
+      <c r="J250" t="n">
+        <v>5</v>
+      </c>
+      <c r="K250" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="n">
+        <v>39250</v>
+      </c>
+      <c r="B251" t="inlineStr">
+        <is>
+          <t>MARKET</t>
+        </is>
+      </c>
+      <c r="C251" t="n">
+        <v>39400</v>
+      </c>
+      <c r="D251" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E251" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F251" t="n">
+        <v>39500</v>
+      </c>
+      <c r="G251" t="n">
+        <v>39300</v>
+      </c>
+      <c r="H251" t="n">
+        <v>4</v>
+      </c>
+      <c r="I251" t="n">
+        <v>2</v>
+      </c>
+      <c r="J251" t="n">
+        <v>5</v>
+      </c>
+      <c r="K251" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="n">
+        <v>39250</v>
+      </c>
+      <c r="B252" t="inlineStr">
+        <is>
+          <t>MARKET</t>
+        </is>
+      </c>
+      <c r="C252" t="n">
+        <v>39400</v>
+      </c>
+      <c r="D252" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E252" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F252" t="n">
+        <v>39500</v>
+      </c>
+      <c r="G252" t="n">
+        <v>39300</v>
+      </c>
+      <c r="H252" t="n">
+        <v>4</v>
+      </c>
+      <c r="I252" t="n">
+        <v>2</v>
+      </c>
+      <c r="J252" t="n">
+        <v>5</v>
+      </c>
+      <c r="K252" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" t="n">
+        <v>39250</v>
+      </c>
+      <c r="B253" t="inlineStr">
+        <is>
+          <t>MARKET</t>
+        </is>
+      </c>
+      <c r="C253" t="n">
+        <v>39400</v>
+      </c>
+      <c r="D253" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E253" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F253" t="n">
+        <v>39500</v>
+      </c>
+      <c r="G253" t="n">
+        <v>39300</v>
+      </c>
+      <c r="H253" t="n">
+        <v>4</v>
+      </c>
+      <c r="I253" t="n">
+        <v>2</v>
+      </c>
+      <c r="J253" t="n">
+        <v>5</v>
+      </c>
+      <c r="K253" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" t="n">
+        <v>39250</v>
+      </c>
+      <c r="B254" t="inlineStr">
+        <is>
+          <t>MARKET</t>
+        </is>
+      </c>
+      <c r="C254" t="n">
+        <v>39400</v>
+      </c>
+      <c r="D254" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E254" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F254" t="n">
+        <v>39500</v>
+      </c>
+      <c r="G254" t="n">
+        <v>39300</v>
+      </c>
+      <c r="H254" t="n">
+        <v>4</v>
+      </c>
+      <c r="I254" t="n">
+        <v>2</v>
+      </c>
+      <c r="J254" t="n">
+        <v>5</v>
+      </c>
+      <c r="K254" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" t="n">
+        <v>39250</v>
+      </c>
+      <c r="B255" t="inlineStr">
+        <is>
+          <t>MARKET</t>
+        </is>
+      </c>
+      <c r="C255" t="n">
+        <v>39400</v>
+      </c>
+      <c r="D255" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E255" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F255" t="n">
+        <v>39500</v>
+      </c>
+      <c r="G255" t="n">
+        <v>39300</v>
+      </c>
+      <c r="H255" t="n">
+        <v>4</v>
+      </c>
+      <c r="I255" t="n">
+        <v>2</v>
+      </c>
+      <c r="J255" t="n">
+        <v>5</v>
+      </c>
+      <c r="K255" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="n">
+        <v>39250</v>
+      </c>
+      <c r="B256" t="inlineStr">
+        <is>
+          <t>MARKET</t>
+        </is>
+      </c>
+      <c r="C256" t="n">
+        <v>39400</v>
+      </c>
+      <c r="D256" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E256" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F256" t="n">
+        <v>39500</v>
+      </c>
+      <c r="G256" t="n">
+        <v>39300</v>
+      </c>
+      <c r="H256" t="n">
+        <v>4</v>
+      </c>
+      <c r="I256" t="n">
+        <v>2</v>
+      </c>
+      <c r="J256" t="n">
+        <v>5</v>
+      </c>
+      <c r="K256" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="n">
+        <v>39250</v>
+      </c>
+      <c r="B257" t="inlineStr">
+        <is>
+          <t>LIMIT</t>
+        </is>
+      </c>
+      <c r="C257" t="n">
+        <v>39400</v>
+      </c>
+      <c r="D257" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E257" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F257" t="n">
+        <v>39500</v>
+      </c>
+      <c r="G257" t="n">
+        <v>39300</v>
+      </c>
+      <c r="H257" t="n">
+        <v>4</v>
+      </c>
+      <c r="I257" t="n">
+        <v>2</v>
+      </c>
+      <c r="J257" t="n">
+        <v>5</v>
+      </c>
+      <c r="K257" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="n">
+        <v>39250</v>
+      </c>
+      <c r="B258" t="inlineStr">
+        <is>
+          <t>LIMIT</t>
+        </is>
+      </c>
+      <c r="C258" t="n">
+        <v>39400</v>
+      </c>
+      <c r="D258" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E258" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F258" t="n">
+        <v>39500</v>
+      </c>
+      <c r="G258" t="n">
+        <v>39300</v>
+      </c>
+      <c r="H258" t="n">
+        <v>4</v>
+      </c>
+      <c r="I258" t="n">
+        <v>2</v>
+      </c>
+      <c r="J258" t="n">
+        <v>5</v>
+      </c>
+      <c r="K258" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" t="n">
+        <v>39250</v>
+      </c>
+      <c r="B259" t="inlineStr">
+        <is>
+          <t>LIMIT</t>
+        </is>
+      </c>
+      <c r="C259" t="n">
+        <v>39400</v>
+      </c>
+      <c r="D259" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E259" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F259" t="n">
+        <v>39500</v>
+      </c>
+      <c r="G259" t="n">
+        <v>39300</v>
+      </c>
+      <c r="H259" t="n">
+        <v>4</v>
+      </c>
+      <c r="I259" t="n">
+        <v>2</v>
+      </c>
+      <c r="J259" t="n">
+        <v>5</v>
+      </c>
+      <c r="K259" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="n">
+        <v>39250</v>
+      </c>
+      <c r="B260" t="inlineStr">
+        <is>
+          <t>LIMIT</t>
+        </is>
+      </c>
+      <c r="C260" t="n">
+        <v>39400</v>
+      </c>
+      <c r="D260" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E260" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F260" t="n">
+        <v>39500</v>
+      </c>
+      <c r="G260" t="n">
+        <v>39300</v>
+      </c>
+      <c r="H260" t="n">
+        <v>4</v>
+      </c>
+      <c r="I260" t="n">
+        <v>2</v>
+      </c>
+      <c r="J260" t="n">
+        <v>5</v>
+      </c>
+      <c r="K260" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="n">
+        <v>39250</v>
+      </c>
+      <c r="B261" t="inlineStr">
+        <is>
+          <t>LIMIT</t>
+        </is>
+      </c>
+      <c r="C261" t="n">
+        <v>39400</v>
+      </c>
+      <c r="D261" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E261" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F261" t="n">
+        <v>39500</v>
+      </c>
+      <c r="G261" t="n">
+        <v>39300</v>
+      </c>
+      <c r="H261" t="n">
+        <v>4</v>
+      </c>
+      <c r="I261" t="n">
+        <v>2</v>
+      </c>
+      <c r="J261" t="n">
+        <v>5</v>
+      </c>
+      <c r="K261" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="n">
+        <v>39250</v>
+      </c>
+      <c r="B262" t="inlineStr">
+        <is>
+          <t>LIMIT</t>
+        </is>
+      </c>
+      <c r="C262" t="n">
+        <v>39400</v>
+      </c>
+      <c r="D262" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E262" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F262" t="n">
+        <v>39500</v>
+      </c>
+      <c r="G262" t="n">
+        <v>39300</v>
+      </c>
+      <c r="H262" t="n">
+        <v>4</v>
+      </c>
+      <c r="I262" t="n">
+        <v>2</v>
+      </c>
+      <c r="J262" t="n">
+        <v>5</v>
+      </c>
+      <c r="K262" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="n">
+        <v>39250</v>
+      </c>
+      <c r="B263" t="inlineStr">
+        <is>
+          <t>LIMIT</t>
+        </is>
+      </c>
+      <c r="C263" t="n">
+        <v>39400</v>
+      </c>
+      <c r="D263" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E263" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F263" t="n">
+        <v>39500</v>
+      </c>
+      <c r="G263" t="n">
+        <v>39300</v>
+      </c>
+      <c r="H263" t="n">
+        <v>4</v>
+      </c>
+      <c r="I263" t="n">
+        <v>2</v>
+      </c>
+      <c r="J263" t="n">
+        <v>5</v>
+      </c>
+      <c r="K263" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" t="n">
+        <v>39250</v>
+      </c>
+      <c r="B264" t="inlineStr">
+        <is>
+          <t>LIMIT</t>
+        </is>
+      </c>
+      <c r="C264" t="n">
+        <v>39400</v>
+      </c>
+      <c r="D264" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E264" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F264" t="n">
+        <v>39500</v>
+      </c>
+      <c r="G264" t="n">
+        <v>39300</v>
+      </c>
+      <c r="H264" t="n">
+        <v>4</v>
+      </c>
+      <c r="I264" t="n">
+        <v>2</v>
+      </c>
+      <c r="J264" t="n">
+        <v>5</v>
+      </c>
+      <c r="K264" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="n">
+        <v>39250</v>
+      </c>
+      <c r="B265" t="inlineStr">
+        <is>
+          <t>LIMIT</t>
+        </is>
+      </c>
+      <c r="C265" t="n">
+        <v>39400</v>
+      </c>
+      <c r="D265" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E265" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F265" t="n">
+        <v>39500</v>
+      </c>
+      <c r="G265" t="n">
+        <v>39300</v>
+      </c>
+      <c r="H265" t="n">
+        <v>4</v>
+      </c>
+      <c r="I265" t="n">
+        <v>2</v>
+      </c>
+      <c r="J265" t="n">
+        <v>5</v>
+      </c>
+      <c r="K265" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" t="n">
+        <v>39250</v>
+      </c>
+      <c r="B266" t="inlineStr">
+        <is>
+          <t>LIMIT</t>
+        </is>
+      </c>
+      <c r="C266" t="n">
+        <v>39400</v>
+      </c>
+      <c r="D266" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E266" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F266" t="n">
+        <v>39500</v>
+      </c>
+      <c r="G266" t="n">
+        <v>39300</v>
+      </c>
+      <c r="H266" t="n">
+        <v>4</v>
+      </c>
+      <c r="I266" t="n">
+        <v>2</v>
+      </c>
+      <c r="J266" t="n">
+        <v>5</v>
+      </c>
+      <c r="K266" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="n">
+        <v>39250</v>
+      </c>
+      <c r="B267" t="inlineStr">
+        <is>
+          <t>LIMIT</t>
+        </is>
+      </c>
+      <c r="C267" t="n">
+        <v>39400</v>
+      </c>
+      <c r="D267" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E267" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F267" t="n">
+        <v>39500</v>
+      </c>
+      <c r="G267" t="n">
+        <v>39300</v>
+      </c>
+      <c r="H267" t="n">
+        <v>4</v>
+      </c>
+      <c r="I267" t="n">
+        <v>2</v>
+      </c>
+      <c r="J267" t="n">
+        <v>5</v>
+      </c>
+      <c r="K267" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" t="n">
+        <v>39250</v>
+      </c>
+      <c r="B268" t="inlineStr">
+        <is>
+          <t>LIMIT</t>
+        </is>
+      </c>
+      <c r="C268" t="n">
+        <v>39400</v>
+      </c>
+      <c r="D268" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E268" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F268" t="n">
+        <v>39500</v>
+      </c>
+      <c r="G268" t="n">
+        <v>39300</v>
+      </c>
+      <c r="H268" t="n">
+        <v>4</v>
+      </c>
+      <c r="I268" t="n">
+        <v>2</v>
+      </c>
+      <c r="J268" t="n">
+        <v>5</v>
+      </c>
+      <c r="K268" t="n">
+        <v>-1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
project completed three order fixed tpsl,auto_square_off working,placing order working check tp_sl logic correct trigger logic correct
</commit_message>
<xml_diff>
--- a/storage/Ibkr.xlsx
+++ b/storage/Ibkr.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K268"/>
+  <dimension ref="A1:K289"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10911,7 +10911,826 @@
         <v>5</v>
       </c>
       <c r="K268" t="n">
-        <v>-1</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" t="n">
+        <v>39250</v>
+      </c>
+      <c r="B269" t="inlineStr">
+        <is>
+          <t>LIMIT</t>
+        </is>
+      </c>
+      <c r="C269" t="n">
+        <v>39400</v>
+      </c>
+      <c r="D269" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E269" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F269" t="n">
+        <v>39500</v>
+      </c>
+      <c r="G269" t="n">
+        <v>39300</v>
+      </c>
+      <c r="H269" t="n">
+        <v>4</v>
+      </c>
+      <c r="I269" t="n">
+        <v>2</v>
+      </c>
+      <c r="J269" t="n">
+        <v>5</v>
+      </c>
+      <c r="K269" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" t="n">
+        <v>39250</v>
+      </c>
+      <c r="B270" t="inlineStr">
+        <is>
+          <t>LIMIT</t>
+        </is>
+      </c>
+      <c r="C270" t="n">
+        <v>39400</v>
+      </c>
+      <c r="D270" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E270" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F270" t="n">
+        <v>39500</v>
+      </c>
+      <c r="G270" t="n">
+        <v>39300</v>
+      </c>
+      <c r="H270" t="n">
+        <v>4</v>
+      </c>
+      <c r="I270" t="n">
+        <v>2</v>
+      </c>
+      <c r="J270" t="n">
+        <v>5</v>
+      </c>
+      <c r="K270" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" t="n">
+        <v>39250</v>
+      </c>
+      <c r="B271" t="inlineStr">
+        <is>
+          <t>LIMIT</t>
+        </is>
+      </c>
+      <c r="C271" t="n">
+        <v>39400</v>
+      </c>
+      <c r="D271" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E271" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F271" t="n">
+        <v>39500</v>
+      </c>
+      <c r="G271" t="n">
+        <v>39300</v>
+      </c>
+      <c r="H271" t="n">
+        <v>4</v>
+      </c>
+      <c r="I271" t="n">
+        <v>2</v>
+      </c>
+      <c r="J271" t="n">
+        <v>5</v>
+      </c>
+      <c r="K271" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" t="n">
+        <v>39250</v>
+      </c>
+      <c r="B272" t="inlineStr">
+        <is>
+          <t>LIMIT</t>
+        </is>
+      </c>
+      <c r="C272" t="n">
+        <v>39400</v>
+      </c>
+      <c r="D272" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E272" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F272" t="n">
+        <v>39500</v>
+      </c>
+      <c r="G272" t="n">
+        <v>39300</v>
+      </c>
+      <c r="H272" t="n">
+        <v>4</v>
+      </c>
+      <c r="I272" t="n">
+        <v>2</v>
+      </c>
+      <c r="J272" t="n">
+        <v>5</v>
+      </c>
+      <c r="K272" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" t="n">
+        <v>39250</v>
+      </c>
+      <c r="B273" t="inlineStr">
+        <is>
+          <t>LIMIT</t>
+        </is>
+      </c>
+      <c r="C273" t="n">
+        <v>39400</v>
+      </c>
+      <c r="D273" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E273" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F273" t="n">
+        <v>39500</v>
+      </c>
+      <c r="G273" t="n">
+        <v>39300</v>
+      </c>
+      <c r="H273" t="n">
+        <v>4</v>
+      </c>
+      <c r="I273" t="n">
+        <v>2</v>
+      </c>
+      <c r="J273" t="n">
+        <v>5</v>
+      </c>
+      <c r="K273" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" t="n">
+        <v>39250</v>
+      </c>
+      <c r="B274" t="inlineStr">
+        <is>
+          <t>LIMIT</t>
+        </is>
+      </c>
+      <c r="C274" t="n">
+        <v>39400</v>
+      </c>
+      <c r="D274" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E274" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F274" t="n">
+        <v>39500</v>
+      </c>
+      <c r="G274" t="n">
+        <v>39300</v>
+      </c>
+      <c r="H274" t="n">
+        <v>4</v>
+      </c>
+      <c r="I274" t="n">
+        <v>2</v>
+      </c>
+      <c r="J274" t="n">
+        <v>5</v>
+      </c>
+      <c r="K274" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" t="n">
+        <v>39250</v>
+      </c>
+      <c r="B275" t="inlineStr">
+        <is>
+          <t>LIMIT</t>
+        </is>
+      </c>
+      <c r="C275" t="n">
+        <v>39400</v>
+      </c>
+      <c r="D275" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E275" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F275" t="n">
+        <v>39500</v>
+      </c>
+      <c r="G275" t="n">
+        <v>39300</v>
+      </c>
+      <c r="H275" t="n">
+        <v>4</v>
+      </c>
+      <c r="I275" t="n">
+        <v>2</v>
+      </c>
+      <c r="J275" t="n">
+        <v>5</v>
+      </c>
+      <c r="K275" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" t="n">
+        <v>39250</v>
+      </c>
+      <c r="B276" t="inlineStr">
+        <is>
+          <t>LIMIT</t>
+        </is>
+      </c>
+      <c r="C276" t="n">
+        <v>39400</v>
+      </c>
+      <c r="D276" t="inlineStr">
+        <is>
+          <t>CE</t>
+        </is>
+      </c>
+      <c r="E276" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F276" t="n">
+        <v>39500</v>
+      </c>
+      <c r="G276" t="n">
+        <v>39300</v>
+      </c>
+      <c r="H276" t="n">
+        <v>4</v>
+      </c>
+      <c r="I276" t="n">
+        <v>2</v>
+      </c>
+      <c r="J276" t="n">
+        <v>5</v>
+      </c>
+      <c r="K276" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" t="n">
+        <v>39400</v>
+      </c>
+      <c r="B277" t="inlineStr">
+        <is>
+          <t>LIMIT</t>
+        </is>
+      </c>
+      <c r="C277" t="n">
+        <v>39470</v>
+      </c>
+      <c r="D277" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E277" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F277" t="n">
+        <v>39530</v>
+      </c>
+      <c r="G277" t="n">
+        <v>39420</v>
+      </c>
+      <c r="H277" t="n">
+        <v>4</v>
+      </c>
+      <c r="I277" t="n">
+        <v>2</v>
+      </c>
+      <c r="J277" t="n">
+        <v>5</v>
+      </c>
+      <c r="K277" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" t="n">
+        <v>39400</v>
+      </c>
+      <c r="B278" t="inlineStr">
+        <is>
+          <t>LIMIT</t>
+        </is>
+      </c>
+      <c r="C278" t="n">
+        <v>39470</v>
+      </c>
+      <c r="D278" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E278" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F278" t="n">
+        <v>39530</v>
+      </c>
+      <c r="G278" t="n">
+        <v>39420</v>
+      </c>
+      <c r="H278" t="n">
+        <v>4</v>
+      </c>
+      <c r="I278" t="n">
+        <v>2</v>
+      </c>
+      <c r="J278" t="n">
+        <v>5</v>
+      </c>
+      <c r="K278" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" t="n">
+        <v>39400</v>
+      </c>
+      <c r="B279" t="inlineStr">
+        <is>
+          <t>LIMIT</t>
+        </is>
+      </c>
+      <c r="C279" t="n">
+        <v>39435</v>
+      </c>
+      <c r="D279" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E279" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F279" t="n">
+        <v>39500</v>
+      </c>
+      <c r="G279" t="n">
+        <v>39380</v>
+      </c>
+      <c r="H279" t="n">
+        <v>4</v>
+      </c>
+      <c r="I279" t="n">
+        <v>2</v>
+      </c>
+      <c r="J279" t="n">
+        <v>5</v>
+      </c>
+      <c r="K279" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" t="n">
+        <v>39400</v>
+      </c>
+      <c r="B280" t="inlineStr">
+        <is>
+          <t>LIMIT</t>
+        </is>
+      </c>
+      <c r="C280" t="n">
+        <v>39425</v>
+      </c>
+      <c r="D280" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E280" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F280" t="n">
+        <v>39500</v>
+      </c>
+      <c r="G280" t="n">
+        <v>39380</v>
+      </c>
+      <c r="H280" t="n">
+        <v>4</v>
+      </c>
+      <c r="I280" t="n">
+        <v>2</v>
+      </c>
+      <c r="J280" t="n">
+        <v>5</v>
+      </c>
+      <c r="K280" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" t="n">
+        <v>39400</v>
+      </c>
+      <c r="B281" t="inlineStr">
+        <is>
+          <t>LIMIT</t>
+        </is>
+      </c>
+      <c r="C281" t="n">
+        <v>39435</v>
+      </c>
+      <c r="D281" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E281" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F281" t="n">
+        <v>39500</v>
+      </c>
+      <c r="G281" t="n">
+        <v>39380</v>
+      </c>
+      <c r="H281" t="n">
+        <v>4</v>
+      </c>
+      <c r="I281" t="n">
+        <v>2</v>
+      </c>
+      <c r="J281" t="n">
+        <v>5</v>
+      </c>
+      <c r="K281" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" t="n">
+        <v>39400</v>
+      </c>
+      <c r="B282" t="inlineStr">
+        <is>
+          <t>LIMIT</t>
+        </is>
+      </c>
+      <c r="C282" t="n">
+        <v>39435</v>
+      </c>
+      <c r="D282" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E282" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F282" t="n">
+        <v>39500</v>
+      </c>
+      <c r="G282" t="n">
+        <v>39380</v>
+      </c>
+      <c r="H282" t="n">
+        <v>4</v>
+      </c>
+      <c r="I282" t="n">
+        <v>2</v>
+      </c>
+      <c r="J282" t="n">
+        <v>5</v>
+      </c>
+      <c r="K282" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" t="n">
+        <v>38400</v>
+      </c>
+      <c r="B283" t="inlineStr">
+        <is>
+          <t>LIMIT</t>
+        </is>
+      </c>
+      <c r="C283" t="n">
+        <v>38455</v>
+      </c>
+      <c r="D283" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E283" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F283" t="n">
+        <v>39500</v>
+      </c>
+      <c r="G283" t="n">
+        <v>39380</v>
+      </c>
+      <c r="H283" t="n">
+        <v>4</v>
+      </c>
+      <c r="I283" t="n">
+        <v>2</v>
+      </c>
+      <c r="J283" t="n">
+        <v>5</v>
+      </c>
+      <c r="K283" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" t="n">
+        <v>38400</v>
+      </c>
+      <c r="B284" t="inlineStr">
+        <is>
+          <t>LIMIT</t>
+        </is>
+      </c>
+      <c r="C284" t="n">
+        <v>38470</v>
+      </c>
+      <c r="D284" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E284" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F284" t="n">
+        <v>38500</v>
+      </c>
+      <c r="G284" t="n">
+        <v>38430</v>
+      </c>
+      <c r="H284" t="n">
+        <v>4</v>
+      </c>
+      <c r="I284" t="n">
+        <v>2</v>
+      </c>
+      <c r="J284" t="n">
+        <v>5</v>
+      </c>
+      <c r="K284" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" t="n">
+        <v>38500</v>
+      </c>
+      <c r="B285" t="inlineStr">
+        <is>
+          <t>LIMIT</t>
+        </is>
+      </c>
+      <c r="C285" t="n">
+        <v>38470</v>
+      </c>
+      <c r="D285" t="inlineStr">
+        <is>
+          <t>CE</t>
+        </is>
+      </c>
+      <c r="E285" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F285" t="n">
+        <v>38430</v>
+      </c>
+      <c r="G285" t="n">
+        <v>38500</v>
+      </c>
+      <c r="H285" t="n">
+        <v>4</v>
+      </c>
+      <c r="I285" t="n">
+        <v>2</v>
+      </c>
+      <c r="J285" t="n">
+        <v>5</v>
+      </c>
+      <c r="K285" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" t="n">
+        <v>38500</v>
+      </c>
+      <c r="B286" t="inlineStr">
+        <is>
+          <t>LIMIT</t>
+        </is>
+      </c>
+      <c r="C286" t="n">
+        <v>38470</v>
+      </c>
+      <c r="D286" t="inlineStr">
+        <is>
+          <t>CE</t>
+        </is>
+      </c>
+      <c r="E286" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F286" t="n">
+        <v>38430</v>
+      </c>
+      <c r="G286" t="n">
+        <v>38500</v>
+      </c>
+      <c r="H286" t="n">
+        <v>4</v>
+      </c>
+      <c r="I286" t="n">
+        <v>2</v>
+      </c>
+      <c r="J286" t="n">
+        <v>5</v>
+      </c>
+      <c r="K286" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" t="n">
+        <v>38450</v>
+      </c>
+      <c r="B287" t="inlineStr">
+        <is>
+          <t>LIMIT</t>
+        </is>
+      </c>
+      <c r="C287" t="n">
+        <v>38470</v>
+      </c>
+      <c r="D287" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E287" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F287" t="n">
+        <v>38600</v>
+      </c>
+      <c r="G287" t="n">
+        <v>38350</v>
+      </c>
+      <c r="H287" t="n">
+        <v>4</v>
+      </c>
+      <c r="I287" t="n">
+        <v>2</v>
+      </c>
+      <c r="J287" t="n">
+        <v>5</v>
+      </c>
+      <c r="K287" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" t="n">
+        <v>38450</v>
+      </c>
+      <c r="B288" t="inlineStr">
+        <is>
+          <t>LIMIT</t>
+        </is>
+      </c>
+      <c r="C288" t="n">
+        <v>38470</v>
+      </c>
+      <c r="D288" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E288" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F288" t="n">
+        <v>38600</v>
+      </c>
+      <c r="G288" t="n">
+        <v>38350</v>
+      </c>
+      <c r="H288" t="n">
+        <v>4</v>
+      </c>
+      <c r="I288" t="n">
+        <v>2</v>
+      </c>
+      <c r="J288" t="n">
+        <v>5</v>
+      </c>
+      <c r="K288" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" t="n">
+        <v>38450</v>
+      </c>
+      <c r="B289" t="inlineStr">
+        <is>
+          <t>LIMIT</t>
+        </is>
+      </c>
+      <c r="C289" t="n">
+        <v>38470</v>
+      </c>
+      <c r="D289" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E289" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F289" t="n">
+        <v>38600</v>
+      </c>
+      <c r="G289" t="n">
+        <v>38350</v>
+      </c>
+      <c r="H289" t="n">
+        <v>4</v>
+      </c>
+      <c r="I289" t="n">
+        <v>2</v>
+      </c>
+      <c r="J289" t="n">
+        <v>5</v>
+      </c>
+      <c r="K289" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
final commit before new changes
</commit_message>
<xml_diff>
--- a/storage/Ibkr.xlsx
+++ b/storage/Ibkr.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K289"/>
+  <dimension ref="A1:K304"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11733,6 +11733,591 @@
         <v>0</v>
       </c>
     </row>
+    <row r="290">
+      <c r="A290" t="n">
+        <v>39000</v>
+      </c>
+      <c r="B290" t="inlineStr">
+        <is>
+          <t>LIMIT</t>
+        </is>
+      </c>
+      <c r="C290" t="n">
+        <v>39100</v>
+      </c>
+      <c r="D290" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E290" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F290" t="n">
+        <v>39300</v>
+      </c>
+      <c r="G290" t="n">
+        <v>38800</v>
+      </c>
+      <c r="H290" t="n">
+        <v>4</v>
+      </c>
+      <c r="I290" t="n">
+        <v>2</v>
+      </c>
+      <c r="J290" t="n">
+        <v>5</v>
+      </c>
+      <c r="K290" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" t="n">
+        <v>39000</v>
+      </c>
+      <c r="B291" t="inlineStr">
+        <is>
+          <t>LIMIT</t>
+        </is>
+      </c>
+      <c r="C291" t="n">
+        <v>39100</v>
+      </c>
+      <c r="D291" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E291" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F291" t="n">
+        <v>39300</v>
+      </c>
+      <c r="G291" t="n">
+        <v>38800</v>
+      </c>
+      <c r="H291" t="n">
+        <v>4</v>
+      </c>
+      <c r="I291" t="n">
+        <v>2</v>
+      </c>
+      <c r="J291" t="n">
+        <v>5</v>
+      </c>
+      <c r="K291" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" t="n">
+        <v>39000</v>
+      </c>
+      <c r="B292" t="inlineStr">
+        <is>
+          <t>LIMIT</t>
+        </is>
+      </c>
+      <c r="C292" t="n">
+        <v>39100</v>
+      </c>
+      <c r="D292" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E292" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F292" t="n">
+        <v>39300</v>
+      </c>
+      <c r="G292" t="n">
+        <v>38800</v>
+      </c>
+      <c r="H292" t="n">
+        <v>4</v>
+      </c>
+      <c r="I292" t="n">
+        <v>2</v>
+      </c>
+      <c r="J292" t="n">
+        <v>5</v>
+      </c>
+      <c r="K292" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" t="n">
+        <v>39300</v>
+      </c>
+      <c r="B293" t="inlineStr">
+        <is>
+          <t>LIMIT</t>
+        </is>
+      </c>
+      <c r="C293" t="n">
+        <v>39100</v>
+      </c>
+      <c r="D293" t="inlineStr">
+        <is>
+          <t>CE</t>
+        </is>
+      </c>
+      <c r="E293" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F293" t="n">
+        <v>39300</v>
+      </c>
+      <c r="G293" t="n">
+        <v>38800</v>
+      </c>
+      <c r="H293" t="n">
+        <v>4</v>
+      </c>
+      <c r="I293" t="n">
+        <v>2</v>
+      </c>
+      <c r="J293" t="n">
+        <v>5</v>
+      </c>
+      <c r="K293" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" t="n">
+        <v>39300</v>
+      </c>
+      <c r="B294" t="inlineStr">
+        <is>
+          <t>LIMIT</t>
+        </is>
+      </c>
+      <c r="C294" t="n">
+        <v>39100</v>
+      </c>
+      <c r="D294" t="inlineStr">
+        <is>
+          <t>CE</t>
+        </is>
+      </c>
+      <c r="E294" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F294" t="n">
+        <v>38800</v>
+      </c>
+      <c r="G294" t="n">
+        <v>39300</v>
+      </c>
+      <c r="H294" t="n">
+        <v>4</v>
+      </c>
+      <c r="I294" t="n">
+        <v>2</v>
+      </c>
+      <c r="J294" t="n">
+        <v>5</v>
+      </c>
+      <c r="K294" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" t="n">
+        <v>38750</v>
+      </c>
+      <c r="B295" t="inlineStr">
+        <is>
+          <t>LIMIT</t>
+        </is>
+      </c>
+      <c r="C295" t="n">
+        <v>38770</v>
+      </c>
+      <c r="D295" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E295" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F295" t="n">
+        <v>38800</v>
+      </c>
+      <c r="G295" t="n">
+        <v>38720</v>
+      </c>
+      <c r="H295" t="n">
+        <v>4</v>
+      </c>
+      <c r="I295" t="n">
+        <v>2</v>
+      </c>
+      <c r="J295" t="n">
+        <v>5</v>
+      </c>
+      <c r="K295" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" t="n">
+        <v>38750</v>
+      </c>
+      <c r="B296" t="inlineStr">
+        <is>
+          <t>LIMIT</t>
+        </is>
+      </c>
+      <c r="C296" t="n">
+        <v>38820</v>
+      </c>
+      <c r="D296" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E296" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F296" t="n">
+        <v>38850</v>
+      </c>
+      <c r="G296" t="n">
+        <v>38790</v>
+      </c>
+      <c r="H296" t="n">
+        <v>4</v>
+      </c>
+      <c r="I296" t="n">
+        <v>2</v>
+      </c>
+      <c r="J296" t="n">
+        <v>5</v>
+      </c>
+      <c r="K296" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" t="n">
+        <v>38850</v>
+      </c>
+      <c r="B297" t="inlineStr">
+        <is>
+          <t>LIMIT</t>
+        </is>
+      </c>
+      <c r="C297" t="n">
+        <v>38835</v>
+      </c>
+      <c r="D297" t="inlineStr">
+        <is>
+          <t>CE</t>
+        </is>
+      </c>
+      <c r="E297" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F297" t="n">
+        <v>38790</v>
+      </c>
+      <c r="G297" t="n">
+        <v>38850</v>
+      </c>
+      <c r="H297" t="n">
+        <v>4</v>
+      </c>
+      <c r="I297" t="n">
+        <v>2</v>
+      </c>
+      <c r="J297" t="n">
+        <v>5</v>
+      </c>
+      <c r="K297" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" t="n">
+        <v>38850</v>
+      </c>
+      <c r="B298" t="inlineStr">
+        <is>
+          <t>LIMIT</t>
+        </is>
+      </c>
+      <c r="C298" t="n">
+        <v>38835</v>
+      </c>
+      <c r="D298" t="inlineStr">
+        <is>
+          <t>CE</t>
+        </is>
+      </c>
+      <c r="E298" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F298" t="n">
+        <v>38800</v>
+      </c>
+      <c r="G298" t="n">
+        <v>38835</v>
+      </c>
+      <c r="H298" t="n">
+        <v>4</v>
+      </c>
+      <c r="I298" t="n">
+        <v>2</v>
+      </c>
+      <c r="J298" t="n">
+        <v>5</v>
+      </c>
+      <c r="K298" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" t="n">
+        <v>38850</v>
+      </c>
+      <c r="B299" t="inlineStr">
+        <is>
+          <t>LIMIT</t>
+        </is>
+      </c>
+      <c r="C299" t="n">
+        <v>38835</v>
+      </c>
+      <c r="D299" t="inlineStr">
+        <is>
+          <t>CE</t>
+        </is>
+      </c>
+      <c r="E299" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F299" t="n">
+        <v>38800</v>
+      </c>
+      <c r="G299" t="n">
+        <v>38835</v>
+      </c>
+      <c r="H299" t="n">
+        <v>4</v>
+      </c>
+      <c r="I299" t="n">
+        <v>2</v>
+      </c>
+      <c r="J299" t="n">
+        <v>5</v>
+      </c>
+      <c r="K299" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" t="n">
+        <v>38850</v>
+      </c>
+      <c r="B300" t="inlineStr">
+        <is>
+          <t>MARKET</t>
+        </is>
+      </c>
+      <c r="C300" t="n">
+        <v>38845</v>
+      </c>
+      <c r="D300" t="inlineStr">
+        <is>
+          <t>CE</t>
+        </is>
+      </c>
+      <c r="E300" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F300" t="n">
+        <v>38835</v>
+      </c>
+      <c r="G300" t="n">
+        <v>38855</v>
+      </c>
+      <c r="H300" t="n">
+        <v>4</v>
+      </c>
+      <c r="I300" t="n">
+        <v>2</v>
+      </c>
+      <c r="J300" t="n">
+        <v>5</v>
+      </c>
+      <c r="K300" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" t="n">
+        <v>39105</v>
+      </c>
+      <c r="B301" t="inlineStr">
+        <is>
+          <t>LIMIT</t>
+        </is>
+      </c>
+      <c r="C301" t="n">
+        <v>39120</v>
+      </c>
+      <c r="D301" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="E301" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F301" t="n">
+        <v>39200</v>
+      </c>
+      <c r="G301" t="n">
+        <v>38900</v>
+      </c>
+      <c r="H301" t="n">
+        <v>4</v>
+      </c>
+      <c r="I301" t="n">
+        <v>2</v>
+      </c>
+      <c r="J301" t="n">
+        <v>5</v>
+      </c>
+      <c r="K301" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" t="n">
+        <v>39135</v>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>LIMIT</t>
+        </is>
+      </c>
+      <c r="C302" t="n">
+        <v>39120</v>
+      </c>
+      <c r="D302" t="inlineStr">
+        <is>
+          <t>CE</t>
+        </is>
+      </c>
+      <c r="E302" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F302" t="n">
+        <v>38800</v>
+      </c>
+      <c r="G302" t="n">
+        <v>39150</v>
+      </c>
+      <c r="H302" t="n">
+        <v>4</v>
+      </c>
+      <c r="I302" t="n">
+        <v>2</v>
+      </c>
+      <c r="J302" t="n">
+        <v>5</v>
+      </c>
+      <c r="K302" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="n">
+        <v>39135</v>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>LIMIT</t>
+        </is>
+      </c>
+      <c r="C303" t="n">
+        <v>39120</v>
+      </c>
+      <c r="D303" t="inlineStr">
+        <is>
+          <t>CE</t>
+        </is>
+      </c>
+      <c r="E303" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F303" t="n">
+        <v>38800</v>
+      </c>
+      <c r="G303" t="n">
+        <v>39150</v>
+      </c>
+      <c r="H303" t="n">
+        <v>4</v>
+      </c>
+      <c r="I303" t="n">
+        <v>2</v>
+      </c>
+      <c r="J303" t="n">
+        <v>5</v>
+      </c>
+      <c r="K303" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="n">
+        <v>39135</v>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>LIMIT</t>
+        </is>
+      </c>
+      <c r="C304" t="n">
+        <v>39120</v>
+      </c>
+      <c r="D304" t="inlineStr">
+        <is>
+          <t>CE</t>
+        </is>
+      </c>
+      <c r="E304" s="6" t="n">
+        <v>45660</v>
+      </c>
+      <c r="F304" t="n">
+        <v>38800</v>
+      </c>
+      <c r="G304" t="n">
+        <v>39150</v>
+      </c>
+      <c r="H304" t="n">
+        <v>4</v>
+      </c>
+      <c r="I304" t="n">
+        <v>2</v>
+      </c>
+      <c r="J304" t="n">
+        <v>5</v>
+      </c>
+      <c r="K304" t="n">
+        <v>-1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
google sheet implemented stoploss implementeed day fixed timestamp fixed pe/ce replaced by buy/sell
</commit_message>
<xml_diff>
--- a/storage/Ibkr.xlsx
+++ b/storage/Ibkr.xlsx
@@ -105,11 +105,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -408,8 +409,8 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A283">
-      <selection activeCell="K304" sqref="K304"/>
+    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A313">
+      <selection activeCell="H323" sqref="H323"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11054,6 +11055,776 @@
         <v>0</v>
       </c>
     </row>
+    <row r="305">
+      <c r="A305">
+        <v>36715</v>
+      </c>
+      <c r="B305" t="s">
+        <v>13</v>
+      </c>
+      <c r="C305">
+        <v>36730</v>
+      </c>
+      <c r="D305" t="s">
+        <v>12</v>
+      </c>
+      <c r="E305" s="2">
+        <v>45660</v>
+      </c>
+      <c r="F305">
+        <v>36750</v>
+      </c>
+      <c r="G305">
+        <v>36700</v>
+      </c>
+      <c r="H305">
+        <v>4</v>
+      </c>
+      <c r="I305">
+        <v>2</v>
+      </c>
+      <c r="J305">
+        <v>5</v>
+      </c>
+      <c r="K305">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306">
+        <v>36705</v>
+      </c>
+      <c r="B306" t="s">
+        <v>13</v>
+      </c>
+      <c r="C306">
+        <v>36710</v>
+      </c>
+      <c r="D306" t="s">
+        <v>12</v>
+      </c>
+      <c r="E306" s="2">
+        <v>45660</v>
+      </c>
+      <c r="F306">
+        <v>36750</v>
+      </c>
+      <c r="G306">
+        <v>36680</v>
+      </c>
+      <c r="H306">
+        <v>4</v>
+      </c>
+      <c r="I306">
+        <v>2</v>
+      </c>
+      <c r="J306">
+        <v>5</v>
+      </c>
+      <c r="K306">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307">
+        <v>36700</v>
+      </c>
+      <c r="B307" t="s">
+        <v>13</v>
+      </c>
+      <c r="C307">
+        <v>36705</v>
+      </c>
+      <c r="D307" t="s">
+        <v>12</v>
+      </c>
+      <c r="E307" s="2">
+        <v>45660</v>
+      </c>
+      <c r="F307">
+        <v>36730</v>
+      </c>
+      <c r="G307">
+        <v>36670</v>
+      </c>
+      <c r="H307">
+        <v>4</v>
+      </c>
+      <c r="I307">
+        <v>2</v>
+      </c>
+      <c r="J307">
+        <v>5</v>
+      </c>
+      <c r="K307">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308">
+        <v>36910</v>
+      </c>
+      <c r="B308" t="s">
+        <v>13</v>
+      </c>
+      <c r="C308">
+        <v>36925</v>
+      </c>
+      <c r="D308" t="s">
+        <v>12</v>
+      </c>
+      <c r="E308" s="2">
+        <v>45661</v>
+      </c>
+      <c r="F308">
+        <v>36950</v>
+      </c>
+      <c r="G308">
+        <v>36860</v>
+      </c>
+      <c r="H308">
+        <v>6</v>
+      </c>
+      <c r="I308">
+        <v>2</v>
+      </c>
+      <c r="J308">
+        <v>5</v>
+      </c>
+      <c r="K308">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309">
+        <v>36850</v>
+      </c>
+      <c r="B309" t="s">
+        <v>13</v>
+      </c>
+      <c r="C309">
+        <v>36870</v>
+      </c>
+      <c r="D309" t="s">
+        <v>12</v>
+      </c>
+      <c r="E309" s="2">
+        <v>45660</v>
+      </c>
+      <c r="F309">
+        <v>36950</v>
+      </c>
+      <c r="G309">
+        <v>36810</v>
+      </c>
+      <c r="H309">
+        <v>6</v>
+      </c>
+      <c r="I309">
+        <v>2</v>
+      </c>
+      <c r="J309">
+        <v>5</v>
+      </c>
+      <c r="K309">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310">
+        <v>36850</v>
+      </c>
+      <c r="B310" t="s">
+        <v>13</v>
+      </c>
+      <c r="C310">
+        <v>36870</v>
+      </c>
+      <c r="D310" t="s">
+        <v>12</v>
+      </c>
+      <c r="E310" s="2">
+        <v>45660</v>
+      </c>
+      <c r="F310">
+        <v>36950</v>
+      </c>
+      <c r="G310">
+        <v>36810</v>
+      </c>
+      <c r="H310">
+        <v>6</v>
+      </c>
+      <c r="I310">
+        <v>2</v>
+      </c>
+      <c r="J310">
+        <v>5</v>
+      </c>
+      <c r="K310">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311">
+        <v>36850</v>
+      </c>
+      <c r="B311" t="s">
+        <v>13</v>
+      </c>
+      <c r="C311">
+        <v>36870</v>
+      </c>
+      <c r="D311" t="s">
+        <v>12</v>
+      </c>
+      <c r="E311" s="2">
+        <v>45660</v>
+      </c>
+      <c r="F311">
+        <v>36950</v>
+      </c>
+      <c r="G311">
+        <v>36810</v>
+      </c>
+      <c r="H311">
+        <v>6</v>
+      </c>
+      <c r="I311">
+        <v>2</v>
+      </c>
+      <c r="J311">
+        <v>5</v>
+      </c>
+      <c r="K311">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312">
+        <v>36850</v>
+      </c>
+      <c r="B312" t="s">
+        <v>13</v>
+      </c>
+      <c r="C312">
+        <v>36870</v>
+      </c>
+      <c r="D312" t="s">
+        <v>12</v>
+      </c>
+      <c r="E312" s="2">
+        <v>45660</v>
+      </c>
+      <c r="F312">
+        <v>36950</v>
+      </c>
+      <c r="G312">
+        <v>36810</v>
+      </c>
+      <c r="H312">
+        <v>6</v>
+      </c>
+      <c r="I312">
+        <v>2</v>
+      </c>
+      <c r="J312">
+        <v>5</v>
+      </c>
+      <c r="K312">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313">
+        <v>36970</v>
+      </c>
+      <c r="B313" t="s">
+        <v>13</v>
+      </c>
+      <c r="C313">
+        <v>37000</v>
+      </c>
+      <c r="D313" t="s">
+        <v>12</v>
+      </c>
+      <c r="E313" s="2">
+        <v>45660</v>
+      </c>
+      <c r="F313">
+        <v>37050</v>
+      </c>
+      <c r="G313">
+        <v>36930</v>
+      </c>
+      <c r="H313">
+        <v>6</v>
+      </c>
+      <c r="I313">
+        <v>2</v>
+      </c>
+      <c r="J313">
+        <v>5</v>
+      </c>
+      <c r="K313">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314">
+        <v>36970</v>
+      </c>
+      <c r="B314" t="s">
+        <v>13</v>
+      </c>
+      <c r="C314">
+        <v>37000</v>
+      </c>
+      <c r="D314" t="s">
+        <v>12</v>
+      </c>
+      <c r="E314" s="2">
+        <v>45660</v>
+      </c>
+      <c r="F314">
+        <v>37050</v>
+      </c>
+      <c r="G314">
+        <v>36930</v>
+      </c>
+      <c r="H314">
+        <v>6</v>
+      </c>
+      <c r="I314">
+        <v>2</v>
+      </c>
+      <c r="J314">
+        <v>5</v>
+      </c>
+      <c r="K314">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315">
+        <v>36790</v>
+      </c>
+      <c r="B315" t="s">
+        <v>13</v>
+      </c>
+      <c r="C315">
+        <v>36810</v>
+      </c>
+      <c r="D315" t="s">
+        <v>12</v>
+      </c>
+      <c r="E315" s="2">
+        <v>45660</v>
+      </c>
+      <c r="F315">
+        <v>36940</v>
+      </c>
+      <c r="G315">
+        <v>36680</v>
+      </c>
+      <c r="H315">
+        <v>4</v>
+      </c>
+      <c r="I315">
+        <v>2</v>
+      </c>
+      <c r="J315">
+        <v>5</v>
+      </c>
+      <c r="K315">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316">
+        <v>36790</v>
+      </c>
+      <c r="B316" t="s">
+        <v>13</v>
+      </c>
+      <c r="C316">
+        <v>36810</v>
+      </c>
+      <c r="D316" t="s">
+        <v>12</v>
+      </c>
+      <c r="E316" s="2">
+        <v>45661</v>
+      </c>
+      <c r="F316">
+        <v>36940</v>
+      </c>
+      <c r="G316">
+        <v>36680</v>
+      </c>
+      <c r="H316">
+        <v>4</v>
+      </c>
+      <c r="I316">
+        <v>2</v>
+      </c>
+      <c r="J316">
+        <v>5</v>
+      </c>
+      <c r="K316">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317">
+        <v>36700</v>
+      </c>
+      <c r="B317" t="s">
+        <v>13</v>
+      </c>
+      <c r="C317">
+        <v>36810</v>
+      </c>
+      <c r="D317" t="s">
+        <v>12</v>
+      </c>
+      <c r="E317" s="2">
+        <v>45661</v>
+      </c>
+      <c r="F317">
+        <v>36940</v>
+      </c>
+      <c r="G317">
+        <v>36680</v>
+      </c>
+      <c r="H317">
+        <v>4</v>
+      </c>
+      <c r="I317">
+        <v>2</v>
+      </c>
+      <c r="J317">
+        <v>5</v>
+      </c>
+      <c r="K317">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318">
+        <v>36700</v>
+      </c>
+      <c r="B318" t="s">
+        <v>13</v>
+      </c>
+      <c r="C318">
+        <v>36740</v>
+      </c>
+      <c r="D318" t="s">
+        <v>12</v>
+      </c>
+      <c r="E318" s="2">
+        <v>45661</v>
+      </c>
+      <c r="F318">
+        <v>36800</v>
+      </c>
+      <c r="G318">
+        <v>36680</v>
+      </c>
+      <c r="H318">
+        <v>4</v>
+      </c>
+      <c r="I318">
+        <v>2</v>
+      </c>
+      <c r="J318">
+        <v>5</v>
+      </c>
+      <c r="K318">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319">
+        <v>36700</v>
+      </c>
+      <c r="B319" t="s">
+        <v>11</v>
+      </c>
+      <c r="C319">
+        <v>36740</v>
+      </c>
+      <c r="D319" t="s">
+        <v>12</v>
+      </c>
+      <c r="E319" s="2">
+        <v>45661</v>
+      </c>
+      <c r="F319">
+        <v>36800</v>
+      </c>
+      <c r="G319">
+        <v>36680</v>
+      </c>
+      <c r="H319">
+        <v>4</v>
+      </c>
+      <c r="I319">
+        <v>2</v>
+      </c>
+      <c r="J319">
+        <v>5</v>
+      </c>
+      <c r="K319">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320">
+        <v>36700</v>
+      </c>
+      <c r="B320" t="s">
+        <v>11</v>
+      </c>
+      <c r="C320">
+        <v>36740</v>
+      </c>
+      <c r="D320" t="s">
+        <v>12</v>
+      </c>
+      <c r="E320" s="2">
+        <v>45661</v>
+      </c>
+      <c r="F320">
+        <v>36800</v>
+      </c>
+      <c r="G320">
+        <v>36680</v>
+      </c>
+      <c r="H320">
+        <v>4</v>
+      </c>
+      <c r="I320">
+        <v>2</v>
+      </c>
+      <c r="J320">
+        <v>5</v>
+      </c>
+      <c r="K320">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321">
+        <v>36880</v>
+      </c>
+      <c r="B321" t="s">
+        <v>11</v>
+      </c>
+      <c r="C321">
+        <v>36880</v>
+      </c>
+      <c r="D321" t="s">
+        <v>14</v>
+      </c>
+      <c r="E321" s="2">
+        <v>45661</v>
+      </c>
+      <c r="F321">
+        <v>36820</v>
+      </c>
+      <c r="G321">
+        <v>36920</v>
+      </c>
+      <c r="H321">
+        <v>4</v>
+      </c>
+      <c r="I321">
+        <v>2</v>
+      </c>
+      <c r="J321">
+        <v>5</v>
+      </c>
+      <c r="K321">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322">
+        <v>36800</v>
+      </c>
+      <c r="B322" t="s">
+        <v>11</v>
+      </c>
+      <c r="C322">
+        <v>36830</v>
+      </c>
+      <c r="D322" t="s">
+        <v>14</v>
+      </c>
+      <c r="E322" s="2">
+        <v>45661</v>
+      </c>
+      <c r="F322">
+        <v>36870</v>
+      </c>
+      <c r="G322">
+        <v>36960</v>
+      </c>
+      <c r="H322">
+        <v>4</v>
+      </c>
+      <c r="I322">
+        <v>2</v>
+      </c>
+      <c r="J322">
+        <v>5</v>
+      </c>
+      <c r="K322">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323">
+        <v>36800</v>
+      </c>
+      <c r="B323" t="s">
+        <v>11</v>
+      </c>
+      <c r="C323">
+        <v>36830</v>
+      </c>
+      <c r="D323" t="s">
+        <v>14</v>
+      </c>
+      <c r="E323" s="2">
+        <v>45661</v>
+      </c>
+      <c r="F323">
+        <v>36870</v>
+      </c>
+      <c r="G323">
+        <v>36960</v>
+      </c>
+      <c r="H323">
+        <v>4</v>
+      </c>
+      <c r="I323">
+        <v>2</v>
+      </c>
+      <c r="J323">
+        <v>5</v>
+      </c>
+      <c r="K323">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324">
+        <v>36800</v>
+      </c>
+      <c r="B324" t="s">
+        <v>11</v>
+      </c>
+      <c r="C324">
+        <v>36830</v>
+      </c>
+      <c r="D324" t="s">
+        <v>14</v>
+      </c>
+      <c r="E324" s="2">
+        <v>45661</v>
+      </c>
+      <c r="F324">
+        <v>36870</v>
+      </c>
+      <c r="G324">
+        <v>36960</v>
+      </c>
+      <c r="H324">
+        <v>4</v>
+      </c>
+      <c r="I324">
+        <v>2</v>
+      </c>
+      <c r="J324">
+        <v>5</v>
+      </c>
+      <c r="K324">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325">
+        <v>36850</v>
+      </c>
+      <c r="B325" t="s">
+        <v>13</v>
+      </c>
+      <c r="C325">
+        <v>36860</v>
+      </c>
+      <c r="D325" t="s">
+        <v>14</v>
+      </c>
+      <c r="E325" s="3">
+        <v>45661</v>
+      </c>
+      <c r="F325">
+        <v>36750</v>
+      </c>
+      <c r="G325">
+        <v>36960</v>
+      </c>
+      <c r="H325">
+        <v>4</v>
+      </c>
+      <c r="I325">
+        <v>2</v>
+      </c>
+      <c r="J325">
+        <v>5</v>
+      </c>
+      <c r="K325">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326">
+        <v>36850</v>
+      </c>
+      <c r="B326" t="s">
+        <v>13</v>
+      </c>
+      <c r="C326">
+        <v>36860</v>
+      </c>
+      <c r="D326" t="s">
+        <v>14</v>
+      </c>
+      <c r="E326" s="3">
+        <v>45661</v>
+      </c>
+      <c r="F326">
+        <v>36750</v>
+      </c>
+      <c r="G326">
+        <v>36960</v>
+      </c>
+      <c r="H326">
+        <v>4</v>
+      </c>
+      <c r="I326">
+        <v>2</v>
+      </c>
+      <c r="J326">
+        <v>5</v>
+      </c>
+      <c r="K326">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>